<commit_message>
Updated the graph of execution times
</commit_message>
<xml_diff>
--- a/2020/analysis/execution times.xlsx
+++ b/2020/analysis/execution times.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ik\git\AdventOfCode\2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ik\git\AdventOfCode\2020\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B238ACE6-DE59-4894-A21C-7F97E7AC2AE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB03E998-8D01-4B54-89E0-8FDE6415C9A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{23AEBC82-DD3C-489D-BC2D-D322F6541D25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="10">
   <si>
     <t>day</t>
   </si>
@@ -46,6 +47,24 @@
   </si>
   <si>
     <t>Part 2</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>of</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Timing</t>
+  </si>
+  <si>
+    <t>init:</t>
+  </si>
+  <si>
+    <t>ns</t>
   </si>
 </sst>
 </file>
@@ -220,10 +239,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -241,33 +260,39 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$7</c:f>
+              <c:f>Sheet1!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.13300000000000001</c:v>
+                  <c:v>0.12790000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.26850000000000002</c:v>
+                  <c:v>0.26569999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.6284000000000001</c:v>
+                  <c:v>1.4305000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.2515</c:v>
+                  <c:v>0.43659999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3962</c:v>
+                  <c:v>0.5242</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.7207999999999999</c:v>
+                  <c:v>2.4479000000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.14510000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -304,10 +329,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -325,33 +350,39 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$7</c:f>
+              <c:f>Sheet1!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.5599999999999999E-2</c:v>
+                  <c:v>1.9099999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.57079999999999997</c:v>
+                  <c:v>0.54059999999999997</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.27E-2</c:v>
+                  <c:v>4.2500000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.743799999999998</c:v>
+                  <c:v>12.691000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.8357</c:v>
+                  <c:v>1.2927</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -388,10 +419,10 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:f>Sheet1!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -409,33 +440,39 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$7</c:f>
+              <c:f>Sheet1!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>2.8099000000000003</c:v>
+                  <c:v>1.1194</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.12179999999999999</c:v>
+                  <c:v>0.16950000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8.0336999999999996</c:v>
+                  <c:v>6.1646999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.5E-3</c:v>
+                  <c:v>5.4999999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.51339999999999997</c:v>
+                  <c:v>0.59609999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1654,10 +1691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC653439-E4E1-46BD-9CBD-A18AF82E67AB}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B13" sqref="B13:D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1681,13 +1718,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.13300000000000001</v>
+        <v>0.12790000000000001</v>
       </c>
       <c r="C2">
-        <v>1.5599999999999999E-2</v>
+        <v>1.9099999999999999E-2</v>
       </c>
       <c r="D2">
-        <v>2.8099000000000003</v>
+        <v>1.1194</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1695,10 +1732,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.26850000000000002</v>
+        <v>0.26569999999999999</v>
       </c>
       <c r="C3">
-        <v>0.57079999999999997</v>
+        <v>0.54059999999999997</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1709,13 +1746,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1.6284000000000001</v>
+        <v>1.4305000000000001</v>
       </c>
       <c r="C4">
-        <v>3.27E-2</v>
+        <v>4.2500000000000003E-2</v>
       </c>
       <c r="D4">
-        <v>0.12179999999999999</v>
+        <v>0.16950000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1723,13 +1760,13 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.2515</v>
+        <v>0.43659999999999999</v>
       </c>
       <c r="C5">
-        <v>10.743799999999998</v>
+        <v>12.691000000000001</v>
       </c>
       <c r="D5">
-        <v>8.0336999999999996</v>
+        <v>6.1646999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1737,13 +1774,13 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.3962</v>
+        <v>0.5242</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1.5E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1751,17 +1788,312 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1.7207999999999999</v>
+        <v>2.4479000000000002</v>
       </c>
       <c r="C7">
-        <v>0.8357</v>
+        <v>1.2927</v>
       </c>
       <c r="D7">
-        <v>0.51339999999999997</v>
+        <v>0.59609999999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.14510000000000001</v>
+      </c>
+      <c r="C8">
+        <v>1E-4</v>
+      </c>
+      <c r="D8">
+        <v>1E-4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB4F610-37CE-40C9-81EE-7142229188EB}">
+  <dimension ref="A1:L7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1">
+        <v>2020</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1">
+        <v>127900</v>
+      </c>
+      <c r="J1">
+        <v>19100</v>
+      </c>
+      <c r="K1">
+        <v>1119400</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>2020</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2">
+        <v>265700</v>
+      </c>
+      <c r="J2">
+        <v>540600</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>2020</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3">
+        <v>1430500</v>
+      </c>
+      <c r="J3">
+        <v>42500</v>
+      </c>
+      <c r="K3">
+        <v>169500</v>
+      </c>
+      <c r="L3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>2020</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4">
+        <v>436600</v>
+      </c>
+      <c r="J4">
+        <v>12691000</v>
+      </c>
+      <c r="K4">
+        <v>6164700</v>
+      </c>
+      <c r="L4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>2020</v>
+      </c>
+      <c r="E5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5">
+        <v>524200</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>5500</v>
+      </c>
+      <c r="L5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>2020</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6">
+        <v>2447900</v>
+      </c>
+      <c r="J6">
+        <v>1292700</v>
+      </c>
+      <c r="K6">
+        <v>596100</v>
+      </c>
+      <c r="L6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>2020</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7">
+        <v>145100</v>
+      </c>
+      <c r="J7">
+        <v>100</v>
+      </c>
+      <c r="K7">
+        <v>100</v>
+      </c>
+      <c r="L7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the running times in the analysis
</commit_message>
<xml_diff>
--- a/2020/analysis/execution times.xlsx
+++ b/2020/analysis/execution times.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ik\git\AdventOfCode\2020\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB03E998-8D01-4B54-89E0-8FDE6415C9A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AFD043-8FE6-468C-92C1-E0FC180F69F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{23AEBC82-DD3C-489D-BC2D-D322F6541D25}"/>
+    <workbookView xWindow="2250" yWindow="1020" windowWidth="22575" windowHeight="14730" xr2:uid="{23AEBC82-DD3C-489D-BC2D-D322F6541D25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -292,7 +292,7 @@
                   <c:v>2.4479000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.14510000000000001</c:v>
+                  <c:v>2.0331999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -382,7 +382,7 @@
                   <c:v>1.2927</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1E-4</c:v>
+                  <c:v>1.9512</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -472,7 +472,7 @@
                   <c:v>0.59609999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1E-4</c:v>
+                  <c:v>1.24E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1694,7 +1694,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:D21"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1802,13 +1802,13 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>0.14510000000000001</v>
+        <v>2.0331999999999999</v>
       </c>
       <c r="C8">
-        <v>1E-4</v>
+        <v>1.9512</v>
       </c>
       <c r="D8">
-        <v>1E-4</v>
+        <v>1.24E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added performance option in run
</commit_message>
<xml_diff>
--- a/2020/analysis/execution times.xlsx
+++ b/2020/analysis/execution times.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ik\git\AdventOfCode\2020\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AFD043-8FE6-468C-92C1-E0FC180F69F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFA4A53-D156-4FBB-8E1C-5814BAF752E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="1020" windowWidth="22575" windowHeight="14730" xr2:uid="{23AEBC82-DD3C-489D-BC2D-D322F6541D25}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{23AEBC82-DD3C-489D-BC2D-D322F6541D25}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>day</t>
   </si>
@@ -47,24 +47,6 @@
   </si>
   <si>
     <t>Part 2</t>
-  </si>
-  <si>
-    <t>Day</t>
-  </si>
-  <si>
-    <t>of</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Timing</t>
-  </si>
-  <si>
-    <t>init:</t>
-  </si>
-  <si>
-    <t>ns</t>
   </si>
 </sst>
 </file>
@@ -237,6 +219,84 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$C$2:$C$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>4.5932000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.7875999999999996E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.190523</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.9574999999999998E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5.2642000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.23102400000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.59222699999999995</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$C$2:$C$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>4.5932000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.7875999999999996E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.190523</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.9574999999999998E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5.2642000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.23102400000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.59222699999999995</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$8</c:f>
@@ -274,25 +334,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.12790000000000001</c:v>
+                  <c:v>7.1585999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.26569999999999999</c:v>
+                  <c:v>0.19689300000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4305000000000001</c:v>
+                  <c:v>1.2259180000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.43659999999999999</c:v>
+                  <c:v>0.22837299999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5242</c:v>
+                  <c:v>0.17044999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.4479000000000002</c:v>
+                  <c:v>1.5276879999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0331999999999999</c:v>
+                  <c:v>4.9923729999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -308,7 +368,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$1</c:f>
+              <c:f>Sheet1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -327,6 +387,84 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$E$2:$E$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>4.4039999999999999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.40146900000000002</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.1285E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.80093499999999995</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4.8999999999999998E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.121304</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.197466</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$E$2:$E$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>4.4039999999999999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.40146900000000002</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.1285E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.80093499999999995</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>4.8999999999999998E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.121304</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.197466</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$8</c:f>
@@ -359,30 +497,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:f>Sheet1!$D$2:$D$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.9099999999999999E-2</c:v>
+                  <c:v>1.9366999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.54059999999999997</c:v>
+                  <c:v>3.2729240000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.2500000000000003E-2</c:v>
+                  <c:v>2.8282999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>12.691000000000001</c:v>
+                  <c:v>5.5518229999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4.0000000000000003E-5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2927</c:v>
+                  <c:v>0.74023399999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9512</c:v>
+                  <c:v>1.2782260000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -398,7 +536,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$1</c:f>
+              <c:f>Sheet1!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -417,6 +555,84 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Sheet1!$G$2:$G$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>0.17524000000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.8000000000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.9381999999999998E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.67028200000000004</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>8.1400000000000005E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.100604</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.4689999999999999E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Sheet1!$G$2:$G$8</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="7"/>
+                  <c:pt idx="0">
+                    <c:v>0.17524000000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>4.8000000000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.9381999999999998E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.67028200000000004</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>8.1400000000000005E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.100604</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.4689999999999999E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:cat>
             <c:numRef>
               <c:f>Sheet1!$A$2:$A$8</c:f>
@@ -449,30 +665,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:f>Sheet1!$F$2:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1.1194</c:v>
+                  <c:v>1.115664</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3.6999999999999998E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.16950000000000001</c:v>
+                  <c:v>0.117711</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.1646999999999998</c:v>
+                  <c:v>4.6642260000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.4999999999999997E-3</c:v>
+                  <c:v>1.207E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.59609999999999996</c:v>
+                  <c:v>0.461117</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.24E-2</c:v>
+                  <c:v>9.6489999999999996E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -580,7 +796,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -606,6 +822,7 @@
         <c:axId val="559693935"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1357,16 +1574,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>395286</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:rowOff>33336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>133349</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1691,124 +1908,187 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC653439-E4E1-46BD-9CBD-A18AF82E67AB}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.12790000000000001</v>
+        <v>7.1585999999999997E-2</v>
       </c>
       <c r="C2">
-        <v>1.9099999999999999E-2</v>
+        <v>4.5932000000000001E-2</v>
       </c>
       <c r="D2">
-        <v>1.1194</v>
+        <v>1.9366999999999999E-2</v>
+      </c>
+      <c r="E2">
+        <v>4.4039999999999999E-3</v>
+      </c>
+      <c r="F2">
+        <v>1.115664</v>
+      </c>
+      <c r="G2">
+        <v>0.17524000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.26569999999999999</v>
+        <v>0.19689300000000001</v>
       </c>
       <c r="C3">
-        <v>0.54059999999999997</v>
+        <v>8.7875999999999996E-2</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>3.2729240000000002</v>
+      </c>
+      <c r="E3">
+        <v>0.40146900000000002</v>
+      </c>
+      <c r="F3">
+        <v>3.6999999999999998E-5</v>
+      </c>
+      <c r="G3">
+        <v>4.8000000000000001E-5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1.4305000000000001</v>
+        <v>1.2259180000000001</v>
       </c>
       <c r="C4">
-        <v>4.2500000000000003E-2</v>
+        <v>0.190523</v>
       </c>
       <c r="D4">
-        <v>0.16950000000000001</v>
+        <v>2.8282999999999999E-2</v>
+      </c>
+      <c r="E4">
+        <v>1.1285E-2</v>
+      </c>
+      <c r="F4">
+        <v>0.117711</v>
+      </c>
+      <c r="G4">
+        <v>2.9381999999999998E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.43659999999999999</v>
+        <v>0.22837299999999999</v>
       </c>
       <c r="C5">
-        <v>12.691000000000001</v>
+        <v>6.9574999999999998E-2</v>
       </c>
       <c r="D5">
-        <v>6.1646999999999998</v>
+        <v>5.5518229999999997</v>
+      </c>
+      <c r="E5">
+        <v>0.80093499999999995</v>
+      </c>
+      <c r="F5">
+        <v>4.6642260000000002</v>
+      </c>
+      <c r="G5">
+        <v>0.67028200000000004</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.5242</v>
+        <v>0.17044999999999999</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>5.2642000000000001E-2</v>
       </c>
       <c r="D6">
-        <v>5.4999999999999997E-3</v>
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="E6">
+        <v>4.8999999999999998E-5</v>
+      </c>
+      <c r="F6">
+        <v>1.207E-3</v>
+      </c>
+      <c r="G6">
+        <v>8.1400000000000005E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>2.4479000000000002</v>
+        <v>1.5276879999999999</v>
       </c>
       <c r="C7">
-        <v>1.2927</v>
+        <v>0.23102400000000001</v>
       </c>
       <c r="D7">
-        <v>0.59609999999999996</v>
+        <v>0.74023399999999995</v>
+      </c>
+      <c r="E7">
+        <v>0.121304</v>
+      </c>
+      <c r="F7">
+        <v>0.461117</v>
+      </c>
+      <c r="G7">
+        <v>0.100604</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>2.0331999999999999</v>
+        <v>4.9923729999999997</v>
       </c>
       <c r="C8">
-        <v>1.9512</v>
+        <v>0.59222699999999995</v>
       </c>
       <c r="D8">
-        <v>1.24E-2</v>
+        <v>1.2782260000000001</v>
+      </c>
+      <c r="E8">
+        <v>0.197466</v>
+      </c>
+      <c r="F8">
+        <v>9.6489999999999996E-3</v>
+      </c>
+      <c r="G8">
+        <v>4.4689999999999999E-3</v>
       </c>
     </row>
   </sheetData>
@@ -1819,278 +2099,341 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB4F610-37CE-40C9-81EE-7142229188EB}">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:K7"/>
+      <selection activeCell="J1" sqref="J1:O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>71586</v>
+      </c>
+      <c r="C1">
+        <v>45932</v>
+      </c>
+      <c r="D1">
+        <v>19367</v>
+      </c>
+      <c r="E1">
+        <v>4404</v>
+      </c>
+      <c r="F1">
+        <v>1115664</v>
+      </c>
+      <c r="G1">
+        <v>175240</v>
+      </c>
+      <c r="J1">
+        <f>+B1/1000000</f>
+        <v>7.1585999999999997E-2</v>
+      </c>
+      <c r="K1">
+        <f t="shared" ref="K1:P7" si="0">+C1/1000000</f>
+        <v>4.5932000000000001E-2</v>
+      </c>
+      <c r="L1">
+        <f t="shared" si="0"/>
+        <v>1.9366999999999999E-2</v>
+      </c>
+      <c r="M1">
+        <f t="shared" si="0"/>
+        <v>4.4039999999999999E-3</v>
+      </c>
+      <c r="N1">
+        <f t="shared" si="0"/>
+        <v>1.115664</v>
+      </c>
+      <c r="O1">
+        <f t="shared" si="0"/>
+        <v>0.17524000000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>196893</v>
+      </c>
+      <c r="C2">
+        <v>87876</v>
+      </c>
+      <c r="D2">
+        <v>3272924</v>
+      </c>
+      <c r="E2">
+        <v>401469</v>
+      </c>
+      <c r="F2">
+        <v>37</v>
+      </c>
+      <c r="G2">
+        <v>48</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ref="J2:J7" si="1">+B2/1000000</f>
+        <v>0.19689300000000001</v>
+      </c>
+      <c r="K2">
+        <f t="shared" si="0"/>
+        <v>8.7875999999999996E-2</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>3.2729240000000002</v>
+      </c>
+      <c r="M2">
+        <f t="shared" si="0"/>
+        <v>0.40146900000000002</v>
+      </c>
+      <c r="N2">
+        <f t="shared" si="0"/>
+        <v>3.6999999999999998E-5</v>
+      </c>
+      <c r="O2">
+        <f t="shared" si="0"/>
+        <v>4.8000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1225918</v>
+      </c>
+      <c r="C3">
+        <v>190523</v>
+      </c>
+      <c r="D3">
+        <v>28283</v>
+      </c>
+      <c r="E3">
+        <v>11285</v>
+      </c>
+      <c r="F3">
+        <v>117711</v>
+      </c>
+      <c r="G3">
+        <v>29382</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="1"/>
+        <v>1.2259180000000001</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>0.190523</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>2.8282999999999999E-2</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>1.1285E-2</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>0.117711</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="0"/>
+        <v>2.9381999999999998E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>4</v>
       </c>
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B4">
+        <v>228373</v>
+      </c>
+      <c r="C4">
+        <v>69575</v>
+      </c>
+      <c r="D4">
+        <v>5551823</v>
+      </c>
+      <c r="E4">
+        <v>800935</v>
+      </c>
+      <c r="F4">
+        <v>4664226</v>
+      </c>
+      <c r="G4">
+        <v>670282</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>0.22837299999999999</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>6.9574999999999998E-2</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>5.5518229999999997</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>0.80093499999999995</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>4.6642260000000002</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>0.67028200000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>5</v>
       </c>
-      <c r="D1">
-        <v>2020</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="B5">
+        <v>170450</v>
+      </c>
+      <c r="C5">
+        <v>52642</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>49</v>
+      </c>
+      <c r="F5">
+        <v>1207</v>
+      </c>
+      <c r="G5">
+        <v>814</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>0.17044999999999999</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>5.2642000000000001E-2</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>4.8999999999999998E-5</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>1.207E-3</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>8.1400000000000005E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B6">
+        <v>1527688</v>
+      </c>
+      <c r="C6">
+        <v>231024</v>
+      </c>
+      <c r="D6">
+        <v>740234</v>
+      </c>
+      <c r="E6">
+        <v>121304</v>
+      </c>
+      <c r="F6">
+        <v>461117</v>
+      </c>
+      <c r="G6">
+        <v>100604</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="1"/>
+        <v>1.5276879999999999</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>0.23102400000000001</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0.74023399999999995</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>0.121304</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>0.461117</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>0.100604</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1">
-        <v>127900</v>
-      </c>
-      <c r="J1">
-        <v>19100</v>
-      </c>
-      <c r="K1">
-        <v>1119400</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>2020</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2">
-        <v>265700</v>
-      </c>
-      <c r="J2">
-        <v>540600</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>2020</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3">
-        <v>1430500</v>
-      </c>
-      <c r="J3">
-        <v>42500</v>
-      </c>
-      <c r="K3">
-        <v>169500</v>
-      </c>
-      <c r="L3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>2020</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4">
-        <v>436600</v>
-      </c>
-      <c r="J4">
-        <v>12691000</v>
-      </c>
-      <c r="K4">
-        <v>6164700</v>
-      </c>
-      <c r="L4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>2020</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5">
-        <v>524200</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>5500</v>
-      </c>
-      <c r="L5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>2020</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6">
-        <v>2447900</v>
-      </c>
-      <c r="J6">
-        <v>1292700</v>
-      </c>
-      <c r="K6">
-        <v>596100</v>
-      </c>
-      <c r="L6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
       <c r="B7">
-        <v>7</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
+        <v>4992373</v>
+      </c>
+      <c r="C7">
+        <v>592227</v>
       </c>
       <c r="D7">
-        <v>2020</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7">
-        <v>145100</v>
+        <v>1278226</v>
+      </c>
+      <c r="E7">
+        <v>197466</v>
+      </c>
+      <c r="F7">
+        <v>9649</v>
+      </c>
+      <c r="G7">
+        <v>4469</v>
       </c>
       <c r="J7">
-        <v>100</v>
+        <f t="shared" si="1"/>
+        <v>4.9923729999999997</v>
       </c>
       <c r="K7">
-        <v>100</v>
-      </c>
-      <c r="L7" t="s">
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>0.59222699999999995</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>1.2782260000000001</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>0.197466</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>9.6489999999999996E-3</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>4.4689999999999999E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the performance analysis
</commit_message>
<xml_diff>
--- a/2020/analysis/execution times.xlsx
+++ b/2020/analysis/execution times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ik\git\AdventOfCode\2020\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFA4A53-D156-4FBB-8E1C-5814BAF752E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{556A5946-7D04-48C9-8F58-335CEF1384E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{23AEBC82-DD3C-489D-BC2D-D322F6541D25}"/>
   </bookViews>
@@ -225,60 +225,66 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$C$2:$C$8</c:f>
+                <c:f>Sheet1!$C$2:$C$9</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="7"/>
+                  <c:ptCount val="8"/>
                   <c:pt idx="0">
-                    <c:v>4.5932000000000001E-2</c:v>
+                    <c:v>2.316E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>8.7875999999999996E-2</c:v>
+                    <c:v>6.6211999999999993E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.190523</c:v>
+                    <c:v>0.14482200000000001</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.9574999999999998E-2</c:v>
+                    <c:v>5.2019999999999997E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.2642000000000001E-2</c:v>
+                    <c:v>4.9805000000000002E-2</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.23102400000000001</c:v>
+                    <c:v>0.15029699999999999</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.59222699999999995</c:v>
+                    <c:v>0.52109000000000005</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>7.5406000000000001E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$C$2:$C$8</c:f>
+                <c:f>Sheet1!$C$2:$C$9</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="7"/>
+                  <c:ptCount val="8"/>
                   <c:pt idx="0">
-                    <c:v>4.5932000000000001E-2</c:v>
+                    <c:v>2.316E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>8.7875999999999996E-2</c:v>
+                    <c:v>6.6211999999999993E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.190523</c:v>
+                    <c:v>0.14482200000000001</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>6.9574999999999998E-2</c:v>
+                    <c:v>5.2019999999999997E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>5.2642000000000001E-2</c:v>
+                    <c:v>4.9805000000000002E-2</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.23102400000000001</c:v>
+                    <c:v>0.15029699999999999</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.59222699999999995</c:v>
+                    <c:v>0.52109000000000005</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>7.5406000000000001E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -299,10 +305,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -323,36 +329,42 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:f>Sheet1!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>7.1585999999999997E-2</c:v>
+                  <c:v>5.8712E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19689300000000001</c:v>
+                  <c:v>0.205125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2259180000000001</c:v>
+                  <c:v>1.234413</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.22837299999999999</c:v>
+                  <c:v>0.20630499999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.17044999999999999</c:v>
+                  <c:v>0.183976</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5276879999999999</c:v>
+                  <c:v>1.5108490000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.9923729999999997</c:v>
+                  <c:v>5.1215549999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.21448</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -393,60 +405,66 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$E$2:$E$8</c:f>
+                <c:f>Sheet1!$E$2:$E$9</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="7"/>
+                  <c:ptCount val="8"/>
                   <c:pt idx="0">
-                    <c:v>4.4039999999999999E-3</c:v>
+                    <c:v>5.6800000000000002E-3</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.40146900000000002</c:v>
+                    <c:v>1.3510219999999999</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.1285E-2</c:v>
+                    <c:v>1.0269E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.80093499999999995</c:v>
+                    <c:v>0.39520499999999997</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4.8999999999999998E-5</c:v>
+                    <c:v>1.163E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.121304</c:v>
+                    <c:v>9.2526999999999998E-2</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.197466</c:v>
+                    <c:v>0.18061199999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1.0736000000000001E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$E$2:$E$8</c:f>
+                <c:f>Sheet1!$E$2:$E$9</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="7"/>
+                  <c:ptCount val="8"/>
                   <c:pt idx="0">
-                    <c:v>4.4039999999999999E-3</c:v>
+                    <c:v>5.6800000000000002E-3</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.40146900000000002</c:v>
+                    <c:v>1.3510219999999999</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>1.1285E-2</c:v>
+                    <c:v>1.0269E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.80093499999999995</c:v>
+                    <c:v>0.39520499999999997</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>4.8999999999999998E-5</c:v>
+                    <c:v>1.163E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.121304</c:v>
+                    <c:v>9.2526999999999998E-2</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.197466</c:v>
+                    <c:v>0.18061199999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1.0736000000000001E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -467,10 +485,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -491,36 +509,42 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$8</c:f>
+              <c:f>Sheet1!$D$2:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.9366999999999999E-2</c:v>
+                  <c:v>1.6763E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.2729240000000002</c:v>
+                  <c:v>2.3959350000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.8282999999999999E-2</c:v>
+                  <c:v>2.7056E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.5518229999999997</c:v>
+                  <c:v>4.8456910000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.0000000000000003E-5</c:v>
+                  <c:v>1.16E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.74023399999999995</c:v>
+                  <c:v>0.75210900000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2782260000000001</c:v>
+                  <c:v>1.3252820000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.5446E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -561,60 +585,66 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>Sheet1!$G$2:$G$8</c:f>
+                <c:f>Sheet1!$G$2:$G$9</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="7"/>
+                  <c:ptCount val="8"/>
                   <c:pt idx="0">
-                    <c:v>0.17524000000000001</c:v>
+                    <c:v>0.112259</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.8000000000000001E-5</c:v>
+                    <c:v>5.0000000000000002E-5</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.9381999999999998E-2</c:v>
+                    <c:v>2.2766999999999999E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.67028200000000004</c:v>
+                    <c:v>0.33945199999999998</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>8.1400000000000005E-4</c:v>
+                    <c:v>1.9289999999999999E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.100604</c:v>
+                    <c:v>8.0642000000000005E-2</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>4.4689999999999999E-3</c:v>
+                    <c:v>4.2300000000000003E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5.3608999999999997E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>Sheet1!$G$2:$G$8</c:f>
+                <c:f>Sheet1!$G$2:$G$9</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="7"/>
+                  <c:ptCount val="8"/>
                   <c:pt idx="0">
-                    <c:v>0.17524000000000001</c:v>
+                    <c:v>0.112259</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>4.8000000000000001E-5</c:v>
+                    <c:v>5.0000000000000002E-5</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.9381999999999998E-2</c:v>
+                    <c:v>2.2766999999999999E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.67028200000000004</c:v>
+                    <c:v>0.33945199999999998</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>8.1400000000000005E-4</c:v>
+                    <c:v>1.9289999999999999E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.100604</c:v>
+                    <c:v>8.0642000000000005E-2</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>4.4689999999999999E-3</c:v>
+                    <c:v>4.2300000000000003E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>5.3608999999999997E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -635,10 +665,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$8</c:f>
+              <c:f>Sheet1!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -659,36 +689,42 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$F$2:$F$8</c:f>
+              <c:f>Sheet1!$F$2:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.115664</c:v>
+                  <c:v>1.0576719999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.6999999999999998E-5</c:v>
+                  <c:v>4.3000000000000002E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.117711</c:v>
+                  <c:v>0.114824</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.6642260000000002</c:v>
+                  <c:v>4.0025240000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.207E-3</c:v>
+                  <c:v>1.323E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.461117</c:v>
+                  <c:v>0.46335599999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.6489999999999996E-3</c:v>
+                  <c:v>1.0035000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.28371299999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1908,10 +1944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC653439-E4E1-46BD-9CBD-A18AF82E67AB}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="Y22" sqref="Y22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1935,22 +1971,22 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>7.1585999999999997E-2</v>
+        <v>5.8712E-2</v>
       </c>
       <c r="C2">
-        <v>4.5932000000000001E-2</v>
+        <v>2.316E-2</v>
       </c>
       <c r="D2">
-        <v>1.9366999999999999E-2</v>
+        <v>1.6763E-2</v>
       </c>
       <c r="E2">
-        <v>4.4039999999999999E-3</v>
+        <v>5.6800000000000002E-3</v>
       </c>
       <c r="F2">
-        <v>1.115664</v>
+        <v>1.0576719999999999</v>
       </c>
       <c r="G2">
-        <v>0.17524000000000001</v>
+        <v>0.112259</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1958,22 +1994,22 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0.19689300000000001</v>
+        <v>0.205125</v>
       </c>
       <c r="C3">
-        <v>8.7875999999999996E-2</v>
+        <v>6.6211999999999993E-2</v>
       </c>
       <c r="D3">
-        <v>3.2729240000000002</v>
+        <v>2.3959350000000001</v>
       </c>
       <c r="E3">
-        <v>0.40146900000000002</v>
+        <v>1.3510219999999999</v>
       </c>
       <c r="F3">
-        <v>3.6999999999999998E-5</v>
+        <v>4.3000000000000002E-5</v>
       </c>
       <c r="G3">
-        <v>4.8000000000000001E-5</v>
+        <v>5.0000000000000002E-5</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1981,22 +2017,22 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1.2259180000000001</v>
+        <v>1.234413</v>
       </c>
       <c r="C4">
-        <v>0.190523</v>
+        <v>0.14482200000000001</v>
       </c>
       <c r="D4">
-        <v>2.8282999999999999E-2</v>
+        <v>2.7056E-2</v>
       </c>
       <c r="E4">
-        <v>1.1285E-2</v>
+        <v>1.0269E-2</v>
       </c>
       <c r="F4">
-        <v>0.117711</v>
+        <v>0.114824</v>
       </c>
       <c r="G4">
-        <v>2.9381999999999998E-2</v>
+        <v>2.2766999999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2004,22 +2040,22 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>0.22837299999999999</v>
+        <v>0.20630499999999999</v>
       </c>
       <c r="C5">
-        <v>6.9574999999999998E-2</v>
+        <v>5.2019999999999997E-2</v>
       </c>
       <c r="D5">
-        <v>5.5518229999999997</v>
+        <v>4.8456910000000004</v>
       </c>
       <c r="E5">
-        <v>0.80093499999999995</v>
+        <v>0.39520499999999997</v>
       </c>
       <c r="F5">
-        <v>4.6642260000000002</v>
+        <v>4.0025240000000002</v>
       </c>
       <c r="G5">
-        <v>0.67028200000000004</v>
+        <v>0.33945199999999998</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2027,22 +2063,22 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>0.17044999999999999</v>
+        <v>0.183976</v>
       </c>
       <c r="C6">
-        <v>5.2642000000000001E-2</v>
+        <v>4.9805000000000002E-2</v>
       </c>
       <c r="D6">
-        <v>4.0000000000000003E-5</v>
+        <v>1.16E-4</v>
       </c>
       <c r="E6">
-        <v>4.8999999999999998E-5</v>
+        <v>1.163E-3</v>
       </c>
       <c r="F6">
-        <v>1.207E-3</v>
+        <v>1.323E-3</v>
       </c>
       <c r="G6">
-        <v>8.1400000000000005E-4</v>
+        <v>1.9289999999999999E-3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2050,22 +2086,22 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1.5276879999999999</v>
+        <v>1.5108490000000001</v>
       </c>
       <c r="C7">
-        <v>0.23102400000000001</v>
+        <v>0.15029699999999999</v>
       </c>
       <c r="D7">
-        <v>0.74023399999999995</v>
+        <v>0.75210900000000003</v>
       </c>
       <c r="E7">
-        <v>0.121304</v>
+        <v>9.2526999999999998E-2</v>
       </c>
       <c r="F7">
-        <v>0.461117</v>
+        <v>0.46335599999999999</v>
       </c>
       <c r="G7">
-        <v>0.100604</v>
+        <v>8.0642000000000005E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2073,22 +2109,45 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>4.9923729999999997</v>
+        <v>5.1215549999999999</v>
       </c>
       <c r="C8">
-        <v>0.59222699999999995</v>
+        <v>0.52109000000000005</v>
       </c>
       <c r="D8">
-        <v>1.2782260000000001</v>
+        <v>1.3252820000000001</v>
       </c>
       <c r="E8">
-        <v>0.197466</v>
+        <v>0.18061199999999999</v>
       </c>
       <c r="F8">
-        <v>9.6489999999999996E-3</v>
+        <v>1.0035000000000001E-2</v>
       </c>
       <c r="G8">
-        <v>4.4689999999999999E-3</v>
+        <v>4.2300000000000003E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.21448</v>
+      </c>
+      <c r="C9">
+        <v>7.5406000000000001E-2</v>
+      </c>
+      <c r="D9">
+        <v>1.5446E-2</v>
+      </c>
+      <c r="E9">
+        <v>1.0736000000000001E-2</v>
+      </c>
+      <c r="F9">
+        <v>0.28371299999999999</v>
+      </c>
+      <c r="G9">
+        <v>5.3608999999999997E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2099,341 +2158,388 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCB4F610-37CE-40C9-81EE-7142229188EB}">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:O7"/>
+      <selection activeCell="I1" sqref="I1:N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1">
-        <v>71586</v>
+        <v>58712</v>
       </c>
       <c r="C1">
-        <v>45932</v>
+        <v>23160</v>
       </c>
       <c r="D1">
-        <v>19367</v>
+        <v>16763</v>
       </c>
       <c r="E1">
-        <v>4404</v>
+        <v>5680</v>
       </c>
       <c r="F1">
-        <v>1115664</v>
+        <v>1057672</v>
       </c>
       <c r="G1">
-        <v>175240</v>
+        <v>112259</v>
+      </c>
+      <c r="I1">
+        <f>+B1/1000000</f>
+        <v>5.8712E-2</v>
       </c>
       <c r="J1">
-        <f>+B1/1000000</f>
-        <v>7.1585999999999997E-2</v>
+        <f t="shared" ref="J1:N8" si="0">+C1/1000000</f>
+        <v>2.316E-2</v>
       </c>
       <c r="K1">
-        <f t="shared" ref="K1:P7" si="0">+C1/1000000</f>
-        <v>4.5932000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>1.6763E-2</v>
       </c>
       <c r="L1">
         <f t="shared" si="0"/>
-        <v>1.9366999999999999E-2</v>
+        <v>5.6800000000000002E-3</v>
       </c>
       <c r="M1">
         <f t="shared" si="0"/>
-        <v>4.4039999999999999E-3</v>
+        <v>1.0576719999999999</v>
       </c>
       <c r="N1">
-        <f t="shared" si="0"/>
-        <v>1.115664</v>
-      </c>
-      <c r="O1">
-        <f t="shared" si="0"/>
-        <v>0.17524000000000001</v>
+        <f>+G1/1000000</f>
+        <v>0.112259</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>196893</v>
+        <v>205125</v>
       </c>
       <c r="C2">
-        <v>87876</v>
+        <v>66212</v>
       </c>
       <c r="D2">
-        <v>3272924</v>
+        <v>2395935</v>
       </c>
       <c r="E2">
-        <v>401469</v>
+        <v>1351022</v>
       </c>
       <c r="F2">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="G2">
-        <v>48</v>
+        <v>50</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:I8" si="1">+B2/1000000</f>
+        <v>0.205125</v>
       </c>
       <c r="J2">
-        <f t="shared" ref="J2:J7" si="1">+B2/1000000</f>
-        <v>0.19689300000000001</v>
+        <f t="shared" si="0"/>
+        <v>6.6211999999999993E-2</v>
       </c>
       <c r="K2">
         <f t="shared" si="0"/>
-        <v>8.7875999999999996E-2</v>
+        <v>2.3959350000000001</v>
       </c>
       <c r="L2">
         <f t="shared" si="0"/>
-        <v>3.2729240000000002</v>
+        <v>1.3510219999999999</v>
       </c>
       <c r="M2">
         <f t="shared" si="0"/>
-        <v>0.40146900000000002</v>
+        <v>4.3000000000000002E-5</v>
       </c>
       <c r="N2">
         <f t="shared" si="0"/>
-        <v>3.6999999999999998E-5</v>
-      </c>
-      <c r="O2">
-        <f t="shared" si="0"/>
-        <v>4.8000000000000001E-5</v>
+        <v>5.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>1225918</v>
+        <v>1234413</v>
       </c>
       <c r="C3">
-        <v>190523</v>
+        <v>144822</v>
       </c>
       <c r="D3">
-        <v>28283</v>
+        <v>27056</v>
       </c>
       <c r="E3">
-        <v>11285</v>
+        <v>10269</v>
       </c>
       <c r="F3">
-        <v>117711</v>
+        <v>114824</v>
       </c>
       <c r="G3">
-        <v>29382</v>
+        <v>22767</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="1"/>
+        <v>1.234413</v>
       </c>
       <c r="J3">
-        <f t="shared" si="1"/>
-        <v>1.2259180000000001</v>
+        <f t="shared" si="0"/>
+        <v>0.14482200000000001</v>
       </c>
       <c r="K3">
         <f t="shared" si="0"/>
-        <v>0.190523</v>
+        <v>2.7056E-2</v>
       </c>
       <c r="L3">
         <f t="shared" si="0"/>
-        <v>2.8282999999999999E-2</v>
+        <v>1.0269E-2</v>
       </c>
       <c r="M3">
         <f t="shared" si="0"/>
-        <v>1.1285E-2</v>
+        <v>0.114824</v>
       </c>
       <c r="N3">
         <f t="shared" si="0"/>
-        <v>0.117711</v>
-      </c>
-      <c r="O3">
-        <f t="shared" si="0"/>
-        <v>2.9381999999999998E-2</v>
+        <v>2.2766999999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4">
-        <v>228373</v>
+        <v>206305</v>
       </c>
       <c r="C4">
-        <v>69575</v>
+        <v>52020</v>
       </c>
       <c r="D4">
-        <v>5551823</v>
+        <v>4845691</v>
       </c>
       <c r="E4">
-        <v>800935</v>
+        <v>395205</v>
       </c>
       <c r="F4">
-        <v>4664226</v>
+        <v>4002524</v>
       </c>
       <c r="G4">
-        <v>670282</v>
+        <v>339452</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>0.20630499999999999</v>
       </c>
       <c r="J4">
-        <f t="shared" si="1"/>
-        <v>0.22837299999999999</v>
+        <f t="shared" si="0"/>
+        <v>5.2019999999999997E-2</v>
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>6.9574999999999998E-2</v>
+        <v>4.8456910000000004</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
-        <v>5.5518229999999997</v>
+        <v>0.39520499999999997</v>
       </c>
       <c r="M4">
         <f t="shared" si="0"/>
-        <v>0.80093499999999995</v>
+        <v>4.0025240000000002</v>
       </c>
       <c r="N4">
         <f t="shared" si="0"/>
-        <v>4.6642260000000002</v>
-      </c>
-      <c r="O4">
-        <f t="shared" si="0"/>
-        <v>0.67028200000000004</v>
+        <v>0.33945199999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5">
-        <v>170450</v>
+        <v>183976</v>
       </c>
       <c r="C5">
-        <v>52642</v>
+        <v>49805</v>
       </c>
       <c r="D5">
-        <v>40</v>
+        <v>116</v>
       </c>
       <c r="E5">
-        <v>49</v>
+        <v>1163</v>
       </c>
       <c r="F5">
-        <v>1207</v>
+        <v>1323</v>
       </c>
       <c r="G5">
-        <v>814</v>
+        <v>1929</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>0.183976</v>
       </c>
       <c r="J5">
-        <f t="shared" si="1"/>
-        <v>0.17044999999999999</v>
+        <f t="shared" si="0"/>
+        <v>4.9805000000000002E-2</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>5.2642000000000001E-2</v>
+        <v>1.16E-4</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>4.0000000000000003E-5</v>
+        <v>1.163E-3</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
-        <v>4.8999999999999998E-5</v>
+        <v>1.323E-3</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>1.207E-3</v>
-      </c>
-      <c r="O5">
-        <f t="shared" si="0"/>
-        <v>8.1400000000000005E-4</v>
+        <v>1.9289999999999999E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>1527688</v>
+        <v>1510849</v>
       </c>
       <c r="C6">
-        <v>231024</v>
+        <v>150297</v>
       </c>
       <c r="D6">
-        <v>740234</v>
+        <v>752109</v>
       </c>
       <c r="E6">
-        <v>121304</v>
+        <v>92527</v>
       </c>
       <c r="F6">
-        <v>461117</v>
+        <v>463356</v>
       </c>
       <c r="G6">
-        <v>100604</v>
+        <v>80642</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>1.5108490000000001</v>
       </c>
       <c r="J6">
-        <f t="shared" si="1"/>
-        <v>1.5276879999999999</v>
+        <f t="shared" si="0"/>
+        <v>0.15029699999999999</v>
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>0.23102400000000001</v>
+        <v>0.75210900000000003</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>0.74023399999999995</v>
+        <v>9.2526999999999998E-2</v>
       </c>
       <c r="M6">
         <f t="shared" si="0"/>
-        <v>0.121304</v>
+        <v>0.46335599999999999</v>
       </c>
       <c r="N6">
         <f t="shared" si="0"/>
-        <v>0.461117</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="0"/>
-        <v>0.100604</v>
+        <v>8.0642000000000005E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7">
-        <v>4992373</v>
+        <v>5121555</v>
       </c>
       <c r="C7">
-        <v>592227</v>
+        <v>521090</v>
       </c>
       <c r="D7">
-        <v>1278226</v>
+        <v>1325282</v>
       </c>
       <c r="E7">
-        <v>197466</v>
+        <v>180612</v>
       </c>
       <c r="F7">
-        <v>9649</v>
+        <v>10035</v>
       </c>
       <c r="G7">
-        <v>4469</v>
+        <v>4230</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>5.1215549999999999</v>
       </c>
       <c r="J7">
+        <f t="shared" si="0"/>
+        <v>0.52109000000000005</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>1.3252820000000001</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>0.18061199999999999</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>1.0035000000000001E-2</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>4.2300000000000003E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>214480</v>
+      </c>
+      <c r="C8">
+        <v>75406</v>
+      </c>
+      <c r="D8">
+        <v>15446</v>
+      </c>
+      <c r="E8">
+        <v>10736</v>
+      </c>
+      <c r="F8">
+        <v>283713</v>
+      </c>
+      <c r="G8">
+        <v>53609</v>
+      </c>
+      <c r="I8">
         <f t="shared" si="1"/>
-        <v>4.9923729999999997</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
-        <v>0.59222699999999995</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="0"/>
-        <v>1.2782260000000001</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="0"/>
-        <v>0.197466</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="0"/>
-        <v>9.6489999999999996E-3</v>
-      </c>
-      <c r="O7">
-        <f t="shared" si="0"/>
-        <v>4.4689999999999999E-3</v>
+        <v>0.21448</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>7.5406000000000001E-2</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>1.5446E-2</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>1.0736000000000001E-2</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>0.28371299999999999</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>5.3608999999999997E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the analysis after day 14
</commit_message>
<xml_diff>
--- a/2020/analysis/execution times.xlsx
+++ b/2020/analysis/execution times.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\arno\git\AdventOfCode\2020\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E712BBCB-9BCC-41D6-921C-39527FB14195}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D55DEE2-DF09-4ECC-B740-C438C81B5730}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{23AEBC82-DD3C-489D-BC2D-D322F6541D25}"/>
   </bookViews>
   <sheets>
     <sheet name="analysis" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Initialization</t>
   </si>
@@ -47,6 +48,21 @@
   </si>
   <si>
     <t>Day</t>
+  </si>
+  <si>
+    <t>+/-</t>
+  </si>
+  <si>
+    <t>ns,</t>
+  </si>
+  <si>
+    <t>p1:</t>
+  </si>
+  <si>
+    <t>p2:</t>
+  </si>
+  <si>
+    <t>ns</t>
   </si>
 </sst>
 </file>
@@ -339,6 +355,9 @@
                   <c:pt idx="12">
                     <c:v>2.2298999999999999E-2</c:v>
                   </c:pt>
+                  <c:pt idx="13">
+                    <c:v>4.8443E-2</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
@@ -386,6 +405,9 @@
                   </c:pt>
                   <c:pt idx="12">
                     <c:v>2.2298999999999999E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>4.8443E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -406,10 +428,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$A$2:$A$14</c:f>
+              <c:f>analysis!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -448,16 +470,19 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$B$2:$B$14</c:f>
+              <c:f>analysis!$B$2:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>8.4697999999999996E-2</c:v>
                 </c:pt>
@@ -496,6 +521,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>6.2486E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.15820000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -579,6 +607,9 @@
                   <c:pt idx="12">
                     <c:v>6.0999999999999999E-5</c:v>
                   </c:pt>
+                  <c:pt idx="13">
+                    <c:v>0.13619200000000001</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
@@ -626,6 +657,9 @@
                   </c:pt>
                   <c:pt idx="12">
                     <c:v>6.0999999999999999E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>0.13619200000000001</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -646,10 +680,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$A$2:$A$14</c:f>
+              <c:f>analysis!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -688,16 +722,19 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$D$2:$D$14</c:f>
+              <c:f>analysis!$D$2:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1.7573999999999999E-2</c:v>
                 </c:pt>
@@ -736,6 +773,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>3.68E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.59872899999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -819,6 +859,9 @@
                   <c:pt idx="12">
                     <c:v>8.2000000000000001E-5</c:v>
                   </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1.8168800000000001</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
@@ -866,6 +909,9 @@
                   </c:pt>
                   <c:pt idx="12">
                     <c:v>8.2000000000000001E-5</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1.8168800000000001</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -886,10 +932,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$A$2:$A$14</c:f>
+              <c:f>analysis!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -928,16 +974,19 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$F$2:$F$14</c:f>
+              <c:f>analysis!$F$2:$F$15</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="13"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>1.097229</c:v>
                 </c:pt>
@@ -976,6 +1025,9 @@
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>7.1500000000000003E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>11.479832999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2198,7 +2250,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="Y26" sqref="Y26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2526,12 +2578,24 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="B15" s="2">
+        <v>0.15820000000000001</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4.8443E-2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.59872899999999996</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.13619200000000001</v>
+      </c>
+      <c r="F15" s="2">
+        <v>11.479832999999999</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1.8168800000000001</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
@@ -2665,17 +2729,17 @@
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <f>+AVERAGE(B2:B26)</f>
-        <v>0.63578392307692311</v>
+        <v>0.60167078571428578</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2">
         <f>+AVERAGE(D2:D26)</f>
-        <v>1.210894153846154</v>
+        <v>1.1671680714285715</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2">
         <f>+AVERAGE(F2:F26)</f>
-        <v>2.0742073076923075</v>
+        <v>2.746037714285714</v>
       </c>
       <c r="G28" s="2"/>
     </row>
@@ -2715,6 +2779,111 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBCE2FE9-9B7E-427F-A660-4FFDCF387270}">
+  <dimension ref="A1:N3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="A3:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>158200</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1">
+        <v>48443</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1">
+        <v>598729</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1">
+        <v>136192</v>
+      </c>
+      <c r="I1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1">
+        <v>11479833</v>
+      </c>
+      <c r="L1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1">
+        <v>1816880</v>
+      </c>
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>158200</v>
+      </c>
+      <c r="B2">
+        <v>48443</v>
+      </c>
+      <c r="C2">
+        <v>598729</v>
+      </c>
+      <c r="D2">
+        <v>136192</v>
+      </c>
+      <c r="E2">
+        <v>11479833</v>
+      </c>
+      <c r="F2">
+        <v>1816880</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>+A2/1000000</f>
+        <v>0.15820000000000001</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:F3" si="0">+B2/1000000</f>
+        <v>4.8443E-2</v>
+      </c>
+      <c r="C3">
+        <f t="shared" si="0"/>
+        <v>0.59872899999999996</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>0.13619200000000001</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>11.479832999999999</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>1.8168800000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A36976-B313-4BEE-90E3-779F1CC50F5B}">
   <dimension ref="A1:M1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated analysis after day 15
</commit_message>
<xml_diff>
--- a/2020/analysis/execution times.xlsx
+++ b/2020/analysis/execution times.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\arno\git\AdventOfCode\2020\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D55DEE2-DF09-4ECC-B740-C438C81B5730}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B94F98-D7AD-4615-967E-C7D0544EE1E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{23AEBC82-DD3C-489D-BC2D-D322F6541D25}"/>
   </bookViews>
   <sheets>
     <sheet name="analysis" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -358,6 +359,9 @@
                   <c:pt idx="13">
                     <c:v>4.8443E-2</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>6.4415549999999997E-5</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
@@ -408,6 +412,9 @@
                   </c:pt>
                   <c:pt idx="13">
                     <c:v>4.8443E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>6.4415549999999997E-5</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -428,10 +435,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$A$2:$A$15</c:f>
+              <c:f>analysis!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -473,16 +480,19 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$B$2:$B$15</c:f>
+              <c:f>analysis!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>8.4697999999999996E-2</c:v>
                 </c:pt>
@@ -524,6 +534,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.15820000000000001</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.1353333333333301E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -610,6 +623,9 @@
                   <c:pt idx="13">
                     <c:v>0.13619200000000001</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>4.2285999999999997E-2</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
@@ -660,6 +676,9 @@
                   </c:pt>
                   <c:pt idx="13">
                     <c:v>0.13619200000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>4.2285999999999997E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -680,10 +699,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$A$2:$A$15</c:f>
+              <c:f>analysis!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -725,16 +744,19 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$D$2:$D$15</c:f>
+              <c:f>analysis!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1.7573999999999999E-2</c:v>
                 </c:pt>
@@ -776,6 +798,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.59872899999999996</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.18688399999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -862,6 +887,9 @@
                   <c:pt idx="13">
                     <c:v>1.8168800000000001</c:v>
                   </c:pt>
+                  <c:pt idx="14">
+                    <c:v>366.99769500000002</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
@@ -912,6 +940,9 @@
                   </c:pt>
                   <c:pt idx="13">
                     <c:v>1.8168800000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>366.99769500000002</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -932,10 +963,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$A$2:$A$15</c:f>
+              <c:f>analysis!$A$2:$A$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -977,16 +1008,19 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$F$2:$F$15</c:f>
+              <c:f>analysis!$F$2:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>1.097229</c:v>
                 </c:pt>
@@ -1028,6 +1062,9 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>11.479832999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>5476.137283</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1039,6 +1076,7 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1161,6 +1199,7 @@
         <c:axId val="559693935"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="16"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1283,6 +1322,45 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-NL"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1291,37 +1369,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-NL"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1921,8 +1968,8 @@
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2250,7 +2297,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y26" sqref="Y26"/>
+      <selection activeCell="W21" sqref="W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2601,12 +2648,24 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
+      <c r="B16" s="2">
+        <v>2.1353333333333301E-4</v>
+      </c>
+      <c r="C16" s="2">
+        <v>6.4415549999999997E-5</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.18688399999999999</v>
+      </c>
+      <c r="E16" s="2">
+        <v>4.2285999999999997E-2</v>
+      </c>
+      <c r="F16" s="2">
+        <v>5476.137283</v>
+      </c>
+      <c r="G16" s="2">
+        <v>366.99769500000002</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
@@ -2729,17 +2788,17 @@
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <f>+AVERAGE(B2:B26)</f>
-        <v>0.60167078571428578</v>
+        <v>0.56157363555555562</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2">
         <f>+AVERAGE(D2:D26)</f>
-        <v>1.1671680714285715</v>
+        <v>1.1018158</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2">
         <f>+AVERAGE(F2:F26)</f>
-        <v>2.746037714285714</v>
+        <v>367.63878740000001</v>
       </c>
       <c r="G28" s="2"/>
     </row>
@@ -2779,6 +2838,77 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F91DEC-A6F9-439E-BB85-4D9003AC1728}">
+  <dimension ref="A1:O1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:O1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>15</v>
+      </c>
+      <c r="B1">
+        <v>50706909</v>
+      </c>
+      <c r="C1">
+        <v>6441555</v>
+      </c>
+      <c r="D1">
+        <v>186884</v>
+      </c>
+      <c r="E1">
+        <v>42286</v>
+      </c>
+      <c r="F1">
+        <v>5476137283</v>
+      </c>
+      <c r="G1">
+        <v>366997695</v>
+      </c>
+      <c r="J1">
+        <f>+B1/1000000</f>
+        <v>50.706909000000003</v>
+      </c>
+      <c r="K1">
+        <f t="shared" ref="K1:O1" si="0">+C1/1000000</f>
+        <v>6.4415550000000001</v>
+      </c>
+      <c r="L1">
+        <f t="shared" si="0"/>
+        <v>0.18688399999999999</v>
+      </c>
+      <c r="M1">
+        <f t="shared" si="0"/>
+        <v>4.2285999999999997E-2</v>
+      </c>
+      <c r="N1">
+        <f t="shared" si="0"/>
+        <v>5476.137283</v>
+      </c>
+      <c r="O1">
+        <f t="shared" si="0"/>
+        <v>366.99769500000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBCE2FE9-9B7E-427F-A660-4FFDCF387270}">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -2883,7 +3013,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A36976-B313-4BEE-90E3-779F1CC50F5B}">
   <dimension ref="A1:M1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Analysis updated after performance increase of day 15 of 2020
</commit_message>
<xml_diff>
--- a/2020/analysis/execution times.xlsx
+++ b/2020/analysis/execution times.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\arno\git\AdventOfCode\2020\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B94F98-D7AD-4615-967E-C7D0544EE1E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAEC285B-D469-495E-AEDD-0FBA9AFF58AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{23AEBC82-DD3C-489D-BC2D-D322F6541D25}"/>
   </bookViews>
   <sheets>
     <sheet name="analysis" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Initialization</t>
   </si>
@@ -64,6 +65,12 @@
   </si>
   <si>
     <t>ns</t>
+  </si>
+  <si>
+    <t>median</t>
+  </si>
+  <si>
+    <t>mean</t>
   </si>
 </sst>
 </file>
@@ -360,7 +367,7 @@
                     <c:v>4.8443E-2</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>6.4415549999999997E-5</c:v>
+                    <c:v>3.8082999999999999E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -414,7 +421,7 @@
                     <c:v>4.8443E-2</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>6.4415549999999997E-5</c:v>
+                    <c:v>3.8082999999999999E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -536,7 +543,7 @@
                   <c:v>0.15820000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.1353333333333301E-4</c:v>
+                  <c:v>0.1983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -624,7 +631,7 @@
                     <c:v>0.13619200000000001</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>4.2285999999999997E-2</c:v>
+                    <c:v>2.9923999999999999E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -678,7 +685,7 @@
                     <c:v>0.13619200000000001</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>4.2285999999999997E-2</c:v>
+                    <c:v>2.9923999999999999E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -800,7 +807,7 @@
                   <c:v>0.59872899999999996</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.18688399999999999</c:v>
+                  <c:v>8.0199999999999994E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -888,7 +895,7 @@
                     <c:v>1.8168800000000001</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>366.99769500000002</c:v>
+                    <c:v>82.883272000000005</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -942,7 +949,7 @@
                     <c:v>1.8168800000000001</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>366.99769500000002</c:v>
+                    <c:v>82.883272000000005</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1064,7 +1071,7 @@
                   <c:v>11.479832999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5476.137283</c:v>
+                  <c:v>2210.9135999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1076,7 +1083,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -2294,10 +2300,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC653439-E4E1-46BD-9CBD-A18AF82E67AB}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W21" sqref="W21"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2649,22 +2655,22 @@
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>2.1353333333333301E-4</v>
+        <v>0.1983</v>
       </c>
       <c r="C16" s="2">
-        <v>6.4415549999999997E-5</v>
+        <v>3.8082999999999999E-2</v>
       </c>
       <c r="D16" s="2">
-        <v>0.18688399999999999</v>
+        <v>8.0199999999999994E-2</v>
       </c>
       <c r="E16" s="2">
-        <v>4.2285999999999997E-2</v>
+        <v>2.9923999999999999E-2</v>
       </c>
       <c r="F16" s="2">
-        <v>5476.137283</v>
+        <v>2210.9135999999999</v>
       </c>
       <c r="G16" s="2">
-        <v>366.99769500000002</v>
+        <v>82.883272000000005</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2786,21 +2792,41 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>10</v>
+      </c>
       <c r="B28" s="2">
         <f>+AVERAGE(B2:B26)</f>
-        <v>0.56157363555555562</v>
+        <v>0.57477940000000005</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2">
         <f>+AVERAGE(D2:D26)</f>
-        <v>1.1018158</v>
+        <v>1.0947035333333335</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2">
         <f>+AVERAGE(F2:F26)</f>
-        <v>367.63878740000001</v>
+        <v>149.95720853333333</v>
       </c>
       <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="2">
+        <f>+MEDIAN(B2:B26)</f>
+        <v>0.180058</v>
+      </c>
+      <c r="D29" s="2">
+        <f>+MEDIAN(D2:D26)</f>
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="F29" s="2">
+        <f>+MEDIAN(F2:F26)</f>
+        <v>0.119423</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2838,6 +2864,65 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61A493B-A071-44C8-977D-BDC58ECB59D8}">
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>198300</v>
+      </c>
+      <c r="B1">
+        <v>38083</v>
+      </c>
+      <c r="C1">
+        <v>80200</v>
+      </c>
+      <c r="D1">
+        <v>29924</v>
+      </c>
+      <c r="E1">
+        <v>2210913600</v>
+      </c>
+      <c r="F1">
+        <v>82883272</v>
+      </c>
+      <c r="H1">
+        <f>+A1/1000000</f>
+        <v>0.1983</v>
+      </c>
+      <c r="I1">
+        <f t="shared" ref="I1:M1" si="0">+B1/1000000</f>
+        <v>3.8082999999999999E-2</v>
+      </c>
+      <c r="J1">
+        <f t="shared" si="0"/>
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="K1">
+        <f t="shared" si="0"/>
+        <v>2.9923999999999999E-2</v>
+      </c>
+      <c r="L1">
+        <f t="shared" si="0"/>
+        <v>2210.9135999999999</v>
+      </c>
+      <c r="M1">
+        <f t="shared" si="0"/>
+        <v>82.883272000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F91DEC-A6F9-439E-BB85-4D9003AC1728}">
   <dimension ref="A1:O1"/>
   <sheetViews>
@@ -2908,7 +2993,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBCE2FE9-9B7E-427F-A660-4FFDCF387270}">
   <dimension ref="A1:N3"/>
   <sheetViews>
@@ -3013,7 +3098,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A36976-B313-4BEE-90E3-779F1CC50F5B}">
   <dimension ref="A1:M1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Analysis updated after performance gain in day 15 of 2020
</commit_message>
<xml_diff>
--- a/2020/analysis/execution times.xlsx
+++ b/2020/analysis/execution times.xlsx
@@ -8,16 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\arno\git\AdventOfCode\2020\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAEC285B-D469-495E-AEDD-0FBA9AFF58AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97E624D-F314-4B7B-B99A-C4661FBA1B67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{23AEBC82-DD3C-489D-BC2D-D322F6541D25}"/>
   </bookViews>
   <sheets>
     <sheet name="analysis" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet4" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Initialization</t>
   </si>
@@ -50,21 +46,6 @@
   </si>
   <si>
     <t>Day</t>
-  </si>
-  <si>
-    <t>+/-</t>
-  </si>
-  <si>
-    <t>ns,</t>
-  </si>
-  <si>
-    <t>p1:</t>
-  </si>
-  <si>
-    <t>p2:</t>
-  </si>
-  <si>
-    <t>ns</t>
   </si>
   <si>
     <t>median</t>
@@ -80,8 +61,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -109,13 +98,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -367,7 +359,7 @@
                     <c:v>4.8443E-2</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>3.8082999999999999E-2</c:v>
+                    <c:v>4.0258000000000002E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -421,7 +413,7 @@
                     <c:v>4.8443E-2</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>3.8082999999999999E-2</c:v>
+                    <c:v>4.0258000000000002E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -543,7 +535,7 @@
                   <c:v>0.15820000000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.1983</c:v>
+                  <c:v>0.22489999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -631,7 +623,7 @@
                     <c:v>0.13619200000000001</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>2.9923999999999999E-2</c:v>
+                    <c:v>3.6999999999999999E-4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -685,7 +677,7 @@
                     <c:v>0.13619200000000001</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>2.9923999999999999E-2</c:v>
+                    <c:v>3.6999999999999999E-4</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -807,7 +799,7 @@
                   <c:v>0.59872899999999996</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>8.0199999999999994E-2</c:v>
+                  <c:v>5.4749999999999998E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -895,7 +887,7 @@
                     <c:v>1.8168800000000001</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>82.883272000000005</c:v>
+                    <c:v>25.593371000000001</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -949,7 +941,7 @@
                     <c:v>1.8168800000000001</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>82.883272000000005</c:v>
+                    <c:v>25.593371000000001</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1071,7 +1063,7 @@
                   <c:v>11.479832999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2210.9135999999999</c:v>
+                  <c:v>890.40279999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1972,8 +1964,8 @@
       <xdr:rowOff>33336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
@@ -2303,7 +2295,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2312,24 +2304,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="2">
@@ -2352,7 +2344,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="2">
@@ -2375,7 +2367,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="B4" s="2">
@@ -2398,7 +2390,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="B5" s="2">
@@ -2421,7 +2413,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="2">
@@ -2444,7 +2436,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="B7" s="2">
@@ -2467,7 +2459,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="B8" s="2">
@@ -2490,7 +2482,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="B9" s="2">
@@ -2513,7 +2505,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="B10" s="2">
@@ -2536,7 +2528,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="B11" s="2">
@@ -2559,7 +2551,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="B12" s="2">
@@ -2582,7 +2574,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="B13" s="2">
@@ -2605,7 +2597,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="2">
@@ -2628,7 +2620,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
       <c r="B15" s="2">
@@ -2651,30 +2643,30 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="2">
-        <v>0.1983</v>
+        <v>0.22489999999999999</v>
       </c>
       <c r="C16" s="2">
-        <v>3.8082999999999999E-2</v>
+        <v>4.0258000000000002E-2</v>
       </c>
       <c r="D16" s="2">
-        <v>8.0199999999999994E-2</v>
+        <v>5.4749999999999998E-3</v>
       </c>
       <c r="E16" s="2">
-        <v>2.9923999999999999E-2</v>
+        <v>3.6999999999999999E-4</v>
       </c>
       <c r="F16" s="2">
-        <v>2210.9135999999999</v>
+        <v>890.40279999999996</v>
       </c>
       <c r="G16" s="2">
-        <v>82.883272000000005</v>
+        <v>25.593371000000001</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="2"/>
@@ -2685,7 +2677,7 @@
       <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="2"/>
@@ -2696,7 +2688,7 @@
       <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="2"/>
@@ -2707,7 +2699,7 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="2"/>
@@ -2718,7 +2710,7 @@
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
       <c r="B21" s="2"/>
@@ -2729,7 +2721,7 @@
       <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
       <c r="B22" s="2"/>
@@ -2740,7 +2732,7 @@
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="2"/>
@@ -2751,7 +2743,7 @@
       <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
       <c r="B24" s="2"/>
@@ -2762,7 +2754,7 @@
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
       <c r="B25" s="2"/>
@@ -2773,7 +2765,7 @@
       <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
       <c r="B26" s="2"/>
@@ -2784,6 +2776,7 @@
       <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -2792,28 +2785,28 @@
       <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
-        <v>10</v>
+      <c r="A28" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="B28" s="2">
         <f>+AVERAGE(B2:B26)</f>
-        <v>0.57477940000000005</v>
+        <v>0.57655273333333334</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2">
         <f>+AVERAGE(D2:D26)</f>
-        <v>1.0947035333333335</v>
+        <v>1.0897218666666668</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2">
         <f>+AVERAGE(F2:F26)</f>
-        <v>149.95720853333333</v>
+        <v>61.923155199999997</v>
       </c>
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>9</v>
+      <c r="A29" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B29" s="2">
         <f>+MEDIAN(B2:B26)</f>
@@ -2821,7 +2814,7 @@
       </c>
       <c r="D29" s="2">
         <f>+MEDIAN(D2:D26)</f>
-        <v>8.0199999999999994E-2</v>
+        <v>2.7345000000000001E-2</v>
       </c>
       <c r="F29" s="2">
         <f>+MEDIAN(F2:F26)</f>
@@ -2859,300 +2852,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61A493B-A071-44C8-977D-BDC58ECB59D8}">
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:M1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>198300</v>
-      </c>
-      <c r="B1">
-        <v>38083</v>
-      </c>
-      <c r="C1">
-        <v>80200</v>
-      </c>
-      <c r="D1">
-        <v>29924</v>
-      </c>
-      <c r="E1">
-        <v>2210913600</v>
-      </c>
-      <c r="F1">
-        <v>82883272</v>
-      </c>
-      <c r="H1">
-        <f>+A1/1000000</f>
-        <v>0.1983</v>
-      </c>
-      <c r="I1">
-        <f t="shared" ref="I1:M1" si="0">+B1/1000000</f>
-        <v>3.8082999999999999E-2</v>
-      </c>
-      <c r="J1">
-        <f t="shared" si="0"/>
-        <v>8.0199999999999994E-2</v>
-      </c>
-      <c r="K1">
-        <f t="shared" si="0"/>
-        <v>2.9923999999999999E-2</v>
-      </c>
-      <c r="L1">
-        <f t="shared" si="0"/>
-        <v>2210.9135999999999</v>
-      </c>
-      <c r="M1">
-        <f t="shared" si="0"/>
-        <v>82.883272000000005</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4F91DEC-A6F9-439E-BB85-4D9003AC1728}">
-  <dimension ref="A1:O1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:O1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>15</v>
-      </c>
-      <c r="B1">
-        <v>50706909</v>
-      </c>
-      <c r="C1">
-        <v>6441555</v>
-      </c>
-      <c r="D1">
-        <v>186884</v>
-      </c>
-      <c r="E1">
-        <v>42286</v>
-      </c>
-      <c r="F1">
-        <v>5476137283</v>
-      </c>
-      <c r="G1">
-        <v>366997695</v>
-      </c>
-      <c r="J1">
-        <f>+B1/1000000</f>
-        <v>50.706909000000003</v>
-      </c>
-      <c r="K1">
-        <f t="shared" ref="K1:O1" si="0">+C1/1000000</f>
-        <v>6.4415550000000001</v>
-      </c>
-      <c r="L1">
-        <f t="shared" si="0"/>
-        <v>0.18688399999999999</v>
-      </c>
-      <c r="M1">
-        <f t="shared" si="0"/>
-        <v>4.2285999999999997E-2</v>
-      </c>
-      <c r="N1">
-        <f t="shared" si="0"/>
-        <v>5476.137283</v>
-      </c>
-      <c r="O1">
-        <f t="shared" si="0"/>
-        <v>366.99769500000002</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBCE2FE9-9B7E-427F-A660-4FFDCF387270}">
-  <dimension ref="A1:N3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="A3:F3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>158200</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1">
-        <v>48443</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1">
-        <v>598729</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1">
-        <v>136192</v>
-      </c>
-      <c r="I1" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" t="s">
-        <v>7</v>
-      </c>
-      <c r="K1">
-        <v>11479833</v>
-      </c>
-      <c r="L1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1">
-        <v>1816880</v>
-      </c>
-      <c r="N1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>158200</v>
-      </c>
-      <c r="B2">
-        <v>48443</v>
-      </c>
-      <c r="C2">
-        <v>598729</v>
-      </c>
-      <c r="D2">
-        <v>136192</v>
-      </c>
-      <c r="E2">
-        <v>11479833</v>
-      </c>
-      <c r="F2">
-        <v>1816880</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <f>+A2/1000000</f>
-        <v>0.15820000000000001</v>
-      </c>
-      <c r="B3">
-        <f t="shared" ref="B3:F3" si="0">+B2/1000000</f>
-        <v>4.8443E-2</v>
-      </c>
-      <c r="C3">
-        <f t="shared" si="0"/>
-        <v>0.59872899999999996</v>
-      </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
-        <v>0.13619200000000001</v>
-      </c>
-      <c r="E3">
-        <f t="shared" si="0"/>
-        <v>11.479832999999999</v>
-      </c>
-      <c r="F3">
-        <f t="shared" si="0"/>
-        <v>1.8168800000000001</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A36976-B313-4BEE-90E3-779F1CC50F5B}">
-  <dimension ref="A1:M1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:M1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>99239</v>
-      </c>
-      <c r="B1">
-        <v>30305</v>
-      </c>
-      <c r="C1">
-        <v>2971</v>
-      </c>
-      <c r="D1">
-        <v>2717</v>
-      </c>
-      <c r="E1">
-        <v>3340</v>
-      </c>
-      <c r="F1">
-        <v>1672</v>
-      </c>
-      <c r="H1">
-        <f>+A1/1000000</f>
-        <v>9.9238999999999994E-2</v>
-      </c>
-      <c r="I1">
-        <f t="shared" ref="I1:M1" si="0">+B1/1000000</f>
-        <v>3.0304999999999999E-2</v>
-      </c>
-      <c r="J1">
-        <f t="shared" si="0"/>
-        <v>2.9710000000000001E-3</v>
-      </c>
-      <c r="K1">
-        <f t="shared" si="0"/>
-        <v>2.7169999999999998E-3</v>
-      </c>
-      <c r="L1">
-        <f t="shared" si="0"/>
-        <v>3.3400000000000001E-3</v>
-      </c>
-      <c r="M1">
-        <f t="shared" si="0"/>
-        <v>1.6720000000000001E-3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated analysis after day 16
</commit_message>
<xml_diff>
--- a/2020/analysis/execution times.xlsx
+++ b/2020/analysis/execution times.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\arno\git\AdventOfCode\2020\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B97E624D-F314-4B7B-B99A-C4661FBA1B67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67D05EA-8BEC-4B75-B3DC-0C173F9EB171}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{23AEBC82-DD3C-489D-BC2D-D322F6541D25}"/>
   </bookViews>
   <sheets>
     <sheet name="analysis" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -361,6 +362,9 @@
                   <c:pt idx="14">
                     <c:v>4.0258000000000002E-2</c:v>
                   </c:pt>
+                  <c:pt idx="15">
+                    <c:v>0.24432300000000001</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
@@ -414,6 +418,9 @@
                   </c:pt>
                   <c:pt idx="14">
                     <c:v>4.0258000000000002E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>0.24432300000000001</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -434,10 +441,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$A$2:$A$16</c:f>
+              <c:f>analysis!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -482,16 +489,19 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$B$2:$B$16</c:f>
+              <c:f>analysis!$B$2:$B$17</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>8.4697999999999996E-2</c:v>
                 </c:pt>
@@ -536,6 +546,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.22489999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.58227399999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -625,6 +638,9 @@
                   <c:pt idx="14">
                     <c:v>3.6999999999999999E-4</c:v>
                   </c:pt>
+                  <c:pt idx="15">
+                    <c:v>8.0731999999999998E-2</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
@@ -678,6 +694,9 @@
                   </c:pt>
                   <c:pt idx="14">
                     <c:v>3.6999999999999999E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>8.0731999999999998E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -698,10 +717,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$A$2:$A$16</c:f>
+              <c:f>analysis!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -746,16 +765,19 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$D$2:$D$16</c:f>
+              <c:f>analysis!$D$2:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>1.7573999999999999E-2</c:v>
                 </c:pt>
@@ -800,6 +822,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>5.4749999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.19489400000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -889,6 +914,9 @@
                   <c:pt idx="14">
                     <c:v>25.593371000000001</c:v>
                   </c:pt>
+                  <c:pt idx="15">
+                    <c:v>0.12117700000000001</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
@@ -942,6 +970,9 @@
                   </c:pt>
                   <c:pt idx="14">
                     <c:v>25.593371000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>0.12117700000000001</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -962,10 +993,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$A$2:$A$16</c:f>
+              <c:f>analysis!$A$2:$A$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1010,16 +1041,19 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$F$2:$F$16</c:f>
+              <c:f>analysis!$F$2:$F$17</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>1.097229</c:v>
                 </c:pt>
@@ -1064,6 +1098,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>890.40279999999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.30002899999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2295,7 +2332,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2669,12 +2706,24 @@
       <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
+      <c r="B17" s="2">
+        <v>0.58227399999999996</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.24432300000000001</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.19489400000000001</v>
+      </c>
+      <c r="E17" s="2">
+        <v>8.0731999999999998E-2</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.30002899999999999</v>
+      </c>
+      <c r="G17" s="2">
+        <v>0.12117700000000001</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
@@ -2790,17 +2839,17 @@
       </c>
       <c r="B28" s="2">
         <f>+AVERAGE(B2:B26)</f>
-        <v>0.57655273333333334</v>
+        <v>0.57691031250000002</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2">
         <f>+AVERAGE(D2:D26)</f>
-        <v>1.0897218666666668</v>
+        <v>1.0337951250000001</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2">
         <f>+AVERAGE(F2:F26)</f>
-        <v>61.923155199999997</v>
+        <v>58.071709812499996</v>
       </c>
       <c r="G28" s="2"/>
     </row>
@@ -2810,15 +2859,15 @@
       </c>
       <c r="B29" s="2">
         <f>+MEDIAN(B2:B26)</f>
-        <v>0.180058</v>
+        <v>0.19082149999999998</v>
       </c>
       <c r="D29" s="2">
         <f>+MEDIAN(D2:D26)</f>
-        <v>2.7345000000000001E-2</v>
+        <v>0.11111950000000001</v>
       </c>
       <c r="F29" s="2">
         <f>+MEDIAN(F2:F26)</f>
-        <v>0.119423</v>
+        <v>0.209726</v>
       </c>
     </row>
   </sheetData>
@@ -2855,4 +2904,63 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654FFB1D-6211-4980-B041-A90B27A14703}">
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>582274</v>
+      </c>
+      <c r="B1">
+        <v>244323</v>
+      </c>
+      <c r="C1">
+        <v>194894</v>
+      </c>
+      <c r="D1">
+        <v>80732</v>
+      </c>
+      <c r="E1">
+        <v>300029</v>
+      </c>
+      <c r="F1">
+        <v>121177</v>
+      </c>
+      <c r="H1">
+        <f>+A1/1000000</f>
+        <v>0.58227399999999996</v>
+      </c>
+      <c r="I1">
+        <f t="shared" ref="I1:M1" si="0">+B1/1000000</f>
+        <v>0.24432300000000001</v>
+      </c>
+      <c r="J1">
+        <f t="shared" si="0"/>
+        <v>0.19489400000000001</v>
+      </c>
+      <c r="K1">
+        <f t="shared" si="0"/>
+        <v>8.0731999999999998E-2</v>
+      </c>
+      <c r="L1">
+        <f t="shared" si="0"/>
+        <v>0.30002899999999999</v>
+      </c>
+      <c r="M1">
+        <f t="shared" si="0"/>
+        <v>0.12117700000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated analysis after refactoring of day 16
</commit_message>
<xml_diff>
--- a/2020/analysis/execution times.xlsx
+++ b/2020/analysis/execution times.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\arno\git\AdventOfCode\2020\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67D05EA-8BEC-4B75-B3DC-0C173F9EB171}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9BEDEA-538A-4A6B-A6CA-9C72CD66DC65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{23AEBC82-DD3C-489D-BC2D-D322F6541D25}"/>
   </bookViews>
   <sheets>
     <sheet name="analysis" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -363,7 +364,7 @@
                     <c:v>4.0258000000000002E-2</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>0.24432300000000001</c:v>
+                    <c:v>0.143709</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -420,7 +421,7 @@
                     <c:v>4.0258000000000002E-2</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>0.24432300000000001</c:v>
+                    <c:v>0.143709</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -548,7 +549,7 @@
                   <c:v>0.22489999999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.58227399999999996</c:v>
+                  <c:v>0.473383</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -639,7 +640,7 @@
                     <c:v>3.6999999999999999E-4</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>8.0731999999999998E-2</c:v>
+                    <c:v>5.416E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -696,7 +697,7 @@
                     <c:v>3.6999999999999999E-4</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>8.0731999999999998E-2</c:v>
+                    <c:v>5.416E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -824,7 +825,7 @@
                   <c:v>5.4749999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.19489400000000001</c:v>
+                  <c:v>0.179065</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -915,7 +916,7 @@
                     <c:v>25.593371000000001</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>0.12117700000000001</c:v>
+                    <c:v>0.143015</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -972,7 +973,7 @@
                     <c:v>25.593371000000001</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>0.12117700000000001</c:v>
+                    <c:v>0.143015</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -1100,7 +1101,7 @@
                   <c:v>890.40279999999996</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.30002899999999999</c:v>
+                  <c:v>0.49242999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2332,7 +2333,7 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2707,22 +2708,22 @@
         <v>16</v>
       </c>
       <c r="B17" s="2">
-        <v>0.58227399999999996</v>
+        <v>0.473383</v>
       </c>
       <c r="C17" s="2">
-        <v>0.24432300000000001</v>
+        <v>0.143709</v>
       </c>
       <c r="D17" s="2">
-        <v>0.19489400000000001</v>
+        <v>0.179065</v>
       </c>
       <c r="E17" s="2">
-        <v>8.0731999999999998E-2</v>
+        <v>5.416E-2</v>
       </c>
       <c r="F17" s="2">
-        <v>0.30002899999999999</v>
+        <v>0.49242999999999998</v>
       </c>
       <c r="G17" s="2">
-        <v>0.12117700000000001</v>
+        <v>0.143015</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2839,17 +2840,17 @@
       </c>
       <c r="B28" s="2">
         <f>+AVERAGE(B2:B26)</f>
-        <v>0.57691031250000002</v>
+        <v>0.57010462500000003</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2">
         <f>+AVERAGE(D2:D26)</f>
-        <v>1.0337951250000001</v>
+        <v>1.0328058125000001</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2">
         <f>+AVERAGE(F2:F26)</f>
-        <v>58.071709812499996</v>
+        <v>58.083734874999998</v>
       </c>
       <c r="G28" s="2"/>
     </row>
@@ -2863,11 +2864,11 @@
       </c>
       <c r="D29" s="2">
         <f>+MEDIAN(D2:D26)</f>
-        <v>0.11111950000000001</v>
+        <v>0.10320499999999999</v>
       </c>
       <c r="F29" s="2">
         <f>+MEDIAN(F2:F26)</f>
-        <v>0.209726</v>
+        <v>0.26024349999999996</v>
       </c>
     </row>
   </sheetData>
@@ -2907,6 +2908,65 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E000E53-3210-4B5E-B4E9-4D5038408630}">
+  <dimension ref="A1:M1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:M1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>473383</v>
+      </c>
+      <c r="B1">
+        <v>143709</v>
+      </c>
+      <c r="C1">
+        <v>179065</v>
+      </c>
+      <c r="D1">
+        <v>54160</v>
+      </c>
+      <c r="E1">
+        <v>492430</v>
+      </c>
+      <c r="F1">
+        <v>143015</v>
+      </c>
+      <c r="H1">
+        <f>+A1/1000000</f>
+        <v>0.473383</v>
+      </c>
+      <c r="I1">
+        <f t="shared" ref="I1:M1" si="0">+B1/1000000</f>
+        <v>0.143709</v>
+      </c>
+      <c r="J1">
+        <f t="shared" si="0"/>
+        <v>0.179065</v>
+      </c>
+      <c r="K1">
+        <f t="shared" si="0"/>
+        <v>5.416E-2</v>
+      </c>
+      <c r="L1">
+        <f t="shared" si="0"/>
+        <v>0.49242999999999998</v>
+      </c>
+      <c r="M1">
+        <f t="shared" si="0"/>
+        <v>0.143015</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654FFB1D-6211-4980-B041-A90B27A14703}">
   <dimension ref="A1:M1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Analysis updated after day 17 of 2020
</commit_message>
<xml_diff>
--- a/2020/analysis/execution times.xlsx
+++ b/2020/analysis/execution times.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\arno\git\AdventOfCode\2020\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9BEDEA-538A-4A6B-A6CA-9C72CD66DC65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15249878-833A-4E62-9C65-3B6FB2DD3817}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{23AEBC82-DD3C-489D-BC2D-D322F6541D25}"/>
   </bookViews>
   <sheets>
     <sheet name="analysis" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Initialization</t>
   </si>
@@ -55,15 +57,42 @@
   <si>
     <t>mean</t>
   </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Init</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Runtime in </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ms</t>
+    </r>
+  </si>
+  <si>
+    <t>Percentage of total runtime</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +108,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -88,7 +148,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -96,27 +156,213 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -289,7 +535,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>analysis!$B$1</c:f>
+              <c:f>analysis!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -314,114 +560,120 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>analysis!$C$2:$C$26</c:f>
+                <c:f>analysis!$C$3:$C$27</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="25"/>
                   <c:pt idx="0">
-                    <c:v>3.7581000000000003E-2</c:v>
+                    <c:v>4.4950999999999998E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.6783E-2</c:v>
+                    <c:v>2.6047000000000001E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.21666099999999999</c:v>
+                    <c:v>0.13864099999999999</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.4775999999999995E-2</c:v>
+                    <c:v>5.2528999999999999E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>8.7070999999999996E-2</c:v>
+                    <c:v>3.0669999999999999E-2</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.41001500000000002</c:v>
+                    <c:v>0.201547</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>1.1107629999999999</c:v>
+                    <c:v>0.85814000000000001</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>5.9840999999999998E-2</c:v>
+                    <c:v>9.5376000000000002E-2</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>7.2169999999999998E-2</c:v>
+                    <c:v>3.9844999999999998E-2</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>4.8404999999999997E-2</c:v>
+                    <c:v>1.9736E-2</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>7.5594999999999996E-2</c:v>
+                    <c:v>4.4547000000000003E-2</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>3.0304999999999999E-2</c:v>
+                    <c:v>2.3973999999999999E-2</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>2.2298999999999999E-2</c:v>
+                    <c:v>1.8241E-2</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>4.8443E-2</c:v>
+                    <c:v>4.2792999999999998E-2</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>4.0258000000000002E-2</c:v>
+                    <c:v>5.5454000000000003E-2</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>0.143709</c:v>
+                    <c:v>0.101872</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>4.0571999999999997E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>analysis!$C$2:$C$26</c:f>
+                <c:f>analysis!$C$3:$C$27</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="25"/>
                   <c:pt idx="0">
-                    <c:v>3.7581000000000003E-2</c:v>
+                    <c:v>4.4950999999999998E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.6783E-2</c:v>
+                    <c:v>2.6047000000000001E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.21666099999999999</c:v>
+                    <c:v>0.13864099999999999</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>7.4775999999999995E-2</c:v>
+                    <c:v>5.2528999999999999E-2</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>8.7070999999999996E-2</c:v>
+                    <c:v>3.0669999999999999E-2</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.41001500000000002</c:v>
+                    <c:v>0.201547</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>1.1107629999999999</c:v>
+                    <c:v>0.85814000000000001</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>5.9840999999999998E-2</c:v>
+                    <c:v>9.5376000000000002E-2</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>7.2169999999999998E-2</c:v>
+                    <c:v>3.9844999999999998E-2</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>4.8404999999999997E-2</c:v>
+                    <c:v>1.9736E-2</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>7.5594999999999996E-2</c:v>
+                    <c:v>4.4547000000000003E-2</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>3.0304999999999999E-2</c:v>
+                    <c:v>2.3973999999999999E-2</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>2.2298999999999999E-2</c:v>
+                    <c:v>1.8241E-2</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>4.8443E-2</c:v>
+                    <c:v>4.2792999999999998E-2</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>4.0258000000000002E-2</c:v>
+                    <c:v>5.5454000000000003E-2</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>0.143709</c:v>
+                    <c:v>0.101872</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>4.0571999999999997E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -442,10 +694,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$A$2:$A$17</c:f>
+              <c:f>analysis!$A$3:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -493,63 +745,69 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$B$2:$B$17</c:f>
+              <c:f>analysis!$B$3:$B$19</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>8.4697999999999996E-2</c:v>
+                  <c:v>7.2594000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14172000000000001</c:v>
+                  <c:v>0.12956300000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.100765</c:v>
+                  <c:v>1.0361370000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20830899999999999</c:v>
+                  <c:v>0.18007400000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.20158499999999999</c:v>
+                  <c:v>0.158967</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2000379999999999</c:v>
+                  <c:v>1.0001040000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.5304440000000001</c:v>
+                  <c:v>4.1733029999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.180058</c:v>
+                  <c:v>0.16120200000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.15038899999999999</c:v>
+                  <c:v>0.124458</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.6862999999999996E-2</c:v>
+                  <c:v>6.3532000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.21859700000000001</c:v>
+                  <c:v>0.164463</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.9238999999999994E-2</c:v>
+                  <c:v>0.100412</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.2486E-2</c:v>
+                  <c:v>6.0907999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.15820000000000001</c:v>
+                  <c:v>0.16551199999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.22489999999999999</c:v>
+                  <c:v>0.20652000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.473383</c:v>
+                  <c:v>0.44292999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.12964899999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -565,7 +823,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>analysis!$D$1</c:f>
+              <c:f>analysis!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -590,114 +848,120 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>analysis!$E$2:$E$26</c:f>
+                <c:f>analysis!$E$3:$E$27</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="25"/>
                   <c:pt idx="0">
-                    <c:v>6.2940000000000001E-3</c:v>
+                    <c:v>2.7780000000000001E-3</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.1894E-2</c:v>
+                    <c:v>6.3132999999999995E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>9.665E-3</c:v>
+                    <c:v>5.4200000000000003E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.66945900000000003</c:v>
+                    <c:v>0.59327600000000003</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.2800000000000001E-3</c:v>
+                    <c:v>6.6600000000000003E-4</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.238708</c:v>
+                    <c:v>0.136485</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.35930299999999998</c:v>
+                    <c:v>0.30520599999999998</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>7.2909999999999997E-3</c:v>
+                    <c:v>3.954E-3</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.124418</c:v>
+                    <c:v>7.5705999999999996E-2</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>1.6180000000000001E-3</c:v>
+                    <c:v>1.6659999999999999E-3</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>1.9718659999999999</c:v>
+                    <c:v>1.1707559999999999</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>2.7169999999999998E-3</c:v>
+                    <c:v>2.1879999999999998E-3</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>6.0999999999999999E-5</c:v>
+                    <c:v>6.0000000000000002E-5</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0.13619200000000001</c:v>
+                    <c:v>0.159972</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>3.6999999999999999E-4</c:v>
+                    <c:v>3.2929999999999999E-3</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>5.416E-2</c:v>
+                    <c:v>3.2071000000000002E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>8.8095000000000007E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>analysis!$E$2:$E$26</c:f>
+                <c:f>analysis!$E$3:$E$27</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="25"/>
                   <c:pt idx="0">
-                    <c:v>6.2940000000000001E-3</c:v>
+                    <c:v>2.7780000000000001E-3</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>7.1894E-2</c:v>
+                    <c:v>6.3132999999999995E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>9.665E-3</c:v>
+                    <c:v>5.4200000000000003E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.66945900000000003</c:v>
+                    <c:v>0.59327600000000003</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.2800000000000001E-3</c:v>
+                    <c:v>6.6600000000000003E-4</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.238708</c:v>
+                    <c:v>0.136485</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.35930299999999998</c:v>
+                    <c:v>0.30520599999999998</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>7.2909999999999997E-3</c:v>
+                    <c:v>3.954E-3</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>0.124418</c:v>
+                    <c:v>7.5705999999999996E-2</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>1.6180000000000001E-3</c:v>
+                    <c:v>1.6659999999999999E-3</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>1.9718659999999999</c:v>
+                    <c:v>1.1707559999999999</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>2.7169999999999998E-3</c:v>
+                    <c:v>2.1879999999999998E-3</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>6.0999999999999999E-5</c:v>
+                    <c:v>6.0000000000000002E-5</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0.13619200000000001</c:v>
+                    <c:v>0.159972</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>3.6999999999999999E-4</c:v>
+                    <c:v>3.2929999999999999E-3</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>5.416E-2</c:v>
+                    <c:v>3.2071000000000002E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>8.8095000000000007E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -718,10 +982,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$A$2:$A$17</c:f>
+              <c:f>analysis!$A$3:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -769,63 +1033,69 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$D$2:$D$17</c:f>
+              <c:f>analysis!$D$3:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>1.7573999999999999E-2</c:v>
+                  <c:v>1.6237999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.32290400000000002</c:v>
+                  <c:v>0.34648699999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7345000000000001E-2</c:v>
+                  <c:v>2.5964000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.162385</c:v>
+                  <c:v>2.927076</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.8000000000000001E-4</c:v>
+                  <c:v>3.4900000000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.66286800000000001</c:v>
+                  <c:v>0.55108999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.321518</c:v>
+                  <c:v>1.31497</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.4205000000000001E-2</c:v>
+                  <c:v>1.3526E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.34794000000000003</c:v>
+                  <c:v>0.29507299999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.5899999999999995E-4</c:v>
+                  <c:v>7.0699999999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.8602070000000008</c:v>
+                  <c:v>9.665934</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.9710000000000001E-3</c:v>
+                  <c:v>2.836E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.68E-4</c:v>
+                  <c:v>3.6600000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.59872899999999996</c:v>
+                  <c:v>0.58871200000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.4749999999999998E-3</c:v>
+                  <c:v>6.5399999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.179065</c:v>
+                  <c:v>0.16650699999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.382911</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -841,7 +1111,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>analysis!$F$1</c:f>
+              <c:f>analysis!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -866,114 +1136,120 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>analysis!$G$2:$G$26</c:f>
+                <c:f>analysis!$G$3:$G$27</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="25"/>
                   <c:pt idx="0">
-                    <c:v>0.144288</c:v>
+                    <c:v>9.8209000000000005E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.34E-4</c:v>
+                    <c:v>4.8000000000000001E-5</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.5323999999999999E-2</c:v>
+                    <c:v>1.4442E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.58426</c:v>
+                    <c:v>0.46395399999999998</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.5449999999999999E-3</c:v>
+                    <c:v>1.74E-4</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.135742</c:v>
+                    <c:v>8.5014999999999993E-2</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>5.5370000000000003E-3</c:v>
+                    <c:v>3.803E-3</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.13026699999999999</c:v>
+                    <c:v>0.106699</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>3.1767999999999998E-2</c:v>
+                    <c:v>2.1406999999999999E-2</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>2.836E-3</c:v>
+                    <c:v>1.2340000000000001E-3</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>2.6741980000000001</c:v>
+                    <c:v>3.1570689999999999</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>1.6720000000000001E-3</c:v>
+                    <c:v>3.1020000000000002E-3</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>8.2000000000000001E-5</c:v>
+                    <c:v>1.665E-3</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>1.8168800000000001</c:v>
+                    <c:v>1.2454320000000001</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>25.593371000000001</c:v>
+                    <c:v>16.886956999999999</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>0.143015</c:v>
+                    <c:v>8.3112000000000005E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>1.290351</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>analysis!$G$2:$G$26</c:f>
+                <c:f>analysis!$G$3:$G$27</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="25"/>
                   <c:pt idx="0">
-                    <c:v>0.144288</c:v>
+                    <c:v>9.8209000000000005E-2</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.34E-4</c:v>
+                    <c:v>4.8000000000000001E-5</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>2.5323999999999999E-2</c:v>
+                    <c:v>1.4442E-2</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.58426</c:v>
+                    <c:v>0.46395399999999998</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>1.5449999999999999E-3</c:v>
+                    <c:v>1.74E-4</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.135742</c:v>
+                    <c:v>8.5014999999999993E-2</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>5.5370000000000003E-3</c:v>
+                    <c:v>3.803E-3</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>0.13026699999999999</c:v>
+                    <c:v>0.106699</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>3.1767999999999998E-2</c:v>
+                    <c:v>2.1406999999999999E-2</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>2.836E-3</c:v>
+                    <c:v>1.2340000000000001E-3</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>2.6741980000000001</c:v>
+                    <c:v>3.1570689999999999</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>1.6720000000000001E-3</c:v>
+                    <c:v>3.1020000000000002E-3</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>8.2000000000000001E-5</c:v>
+                    <c:v>1.665E-3</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>1.8168800000000001</c:v>
+                    <c:v>1.2454320000000001</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>25.593371000000001</c:v>
+                    <c:v>16.886956999999999</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>0.143015</c:v>
+                    <c:v>8.3112000000000005E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>1.290351</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -994,10 +1270,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$A$2:$A$17</c:f>
+              <c:f>analysis!$A$3:$A$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1045,63 +1321,69 @@
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$F$2:$F$17</c:f>
+              <c:f>analysis!$F$3:$F$19</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="16"/>
+                <c:ptCount val="17"/>
                 <c:pt idx="0">
-                  <c:v>1.097229</c:v>
+                  <c:v>1.039283</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.5100000000000002E-4</c:v>
+                  <c:v>3.2299999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.119423</c:v>
+                  <c:v>0.112997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6294110000000002</c:v>
+                  <c:v>2.406755</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6919999999999999E-3</c:v>
+                  <c:v>1.354E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.40106399999999998</c:v>
+                  <c:v>0.32652900000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0252000000000001E-2</c:v>
+                  <c:v>9.3240000000000007E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.53528100000000001</c:v>
+                  <c:v>0.52793400000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.5516999999999996E-2</c:v>
+                  <c:v>7.5289999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.709E-3</c:v>
+                  <c:v>1.15E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22.078710999999998</c:v>
+                  <c:v>22.647563000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.3400000000000001E-3</c:v>
+                  <c:v>3.7650000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.1500000000000003E-4</c:v>
+                  <c:v>7.9900000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.479832999999999</c:v>
+                  <c:v>11.132872000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>890.40279999999996</c:v>
+                  <c:v>865.05989999999997</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.49242999999999998</c:v>
+                  <c:v>0.45431300000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10.257724</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1235,7 +1517,7 @@
         <c:axId val="559693935"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="16"/>
+          <c:max val="12"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1996,16 +2278,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>395286</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>3703</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>33336</xdr:rowOff>
+      <xdr:rowOff>4760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>10584</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2028,6 +2310,72 @@
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63D37E0A-4D42-4E43-9B4A-71B691176EF5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1543050" y="619125"/>
+          <a:ext cx="6715125" cy="5743575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2330,575 +2678,994 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC653439-E4E1-46BD-9CBD-A18AF82E67AB}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.140625" style="14"/>
+    <col min="4" max="4" width="9.140625" style="12"/>
+    <col min="6" max="6" width="9.140625" style="12"/>
+    <col min="8" max="8" width="9.140625" style="10"/>
+    <col min="9" max="11" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B1" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+    </row>
+    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B2" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4" t="s">
+      <c r="C2" s="23"/>
+      <c r="D2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4" t="s">
+      <c r="E2" s="25"/>
+      <c r="F2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+      <c r="G2" s="23"/>
+      <c r="H2" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>8.4697999999999996E-2</v>
-      </c>
-      <c r="C2" s="2">
-        <v>3.7581000000000003E-2</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1.7573999999999999E-2</v>
-      </c>
-      <c r="E2" s="2">
-        <v>6.2940000000000001E-3</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1.097229</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0.144288</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="K2" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13">
+        <v>7.2594000000000006E-2</v>
+      </c>
+      <c r="C3" s="4">
+        <v>4.4950999999999998E-2</v>
+      </c>
+      <c r="D3" s="11">
+        <v>1.6237999999999999E-2</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2.7780000000000001E-3</v>
+      </c>
+      <c r="F3" s="11">
+        <v>1.039283</v>
+      </c>
+      <c r="G3" s="4">
+        <v>9.8209000000000005E-2</v>
+      </c>
+      <c r="H3" s="9">
+        <f>+B3+D3+F3</f>
+        <v>1.128115</v>
+      </c>
+      <c r="I3" s="5">
+        <f>+B3/$H3</f>
+        <v>6.4349822491501313E-2</v>
+      </c>
+      <c r="J3" s="5">
+        <f>+D3/H3</f>
+        <v>1.4393922605408137E-2</v>
+      </c>
+      <c r="K3" s="5">
+        <f>+F3/H3</f>
+        <v>0.92125625490309049</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>0.14172000000000001</v>
-      </c>
-      <c r="C3" s="2">
-        <v>5.6783E-2</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0.32290400000000002</v>
-      </c>
-      <c r="E3" s="2">
-        <v>7.1894E-2</v>
-      </c>
-      <c r="F3" s="2">
-        <v>3.5100000000000002E-4</v>
-      </c>
-      <c r="G3" s="2">
-        <v>2.34E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+      <c r="B4" s="13">
+        <v>0.12956300000000001</v>
+      </c>
+      <c r="C4" s="4">
+        <v>2.6047000000000001E-2</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0.34648699999999999</v>
+      </c>
+      <c r="E4" s="4">
+        <v>6.3132999999999995E-2</v>
+      </c>
+      <c r="F4" s="11">
+        <v>3.2299999999999999E-4</v>
+      </c>
+      <c r="G4" s="4">
+        <v>4.8000000000000001E-5</v>
+      </c>
+      <c r="H4" s="9">
+        <f t="shared" ref="H4:H27" si="0">+B4+D4+F4</f>
+        <v>0.47637299999999999</v>
+      </c>
+      <c r="I4" s="5">
+        <f t="shared" ref="I4:I18" si="1">+B4/$H4</f>
+        <v>0.27197805081312337</v>
+      </c>
+      <c r="J4" s="5">
+        <f t="shared" ref="J4:J18" si="2">+D4/H4</f>
+        <v>0.72734390907964974</v>
+      </c>
+      <c r="K4" s="5">
+        <f t="shared" ref="K4:K18" si="3">+F4/H4</f>
+        <v>6.7804010722689997E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
-        <v>1.100765</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0.21666099999999999</v>
-      </c>
-      <c r="D4" s="2">
-        <v>2.7345000000000001E-2</v>
-      </c>
-      <c r="E4" s="2">
-        <v>9.665E-3</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.119423</v>
-      </c>
-      <c r="G4" s="2">
-        <v>2.5323999999999999E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="B5" s="13">
+        <v>1.0361370000000001</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.13864099999999999</v>
+      </c>
+      <c r="D5" s="11">
+        <v>2.5964000000000001E-2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>5.4200000000000003E-3</v>
+      </c>
+      <c r="F5" s="11">
+        <v>0.112997</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1.4442E-2</v>
+      </c>
+      <c r="H5" s="9">
+        <f t="shared" si="0"/>
+        <v>1.1750980000000002</v>
+      </c>
+      <c r="I5" s="5">
+        <f t="shared" si="1"/>
+        <v>0.88174518210396058</v>
+      </c>
+      <c r="J5" s="5">
+        <f t="shared" si="2"/>
+        <v>2.2095178444691419E-2</v>
+      </c>
+      <c r="K5" s="5">
+        <f t="shared" si="3"/>
+        <v>9.6159639451347867E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <v>0.20830899999999999</v>
-      </c>
-      <c r="C5" s="2">
-        <v>7.4775999999999995E-2</v>
-      </c>
-      <c r="D5" s="2">
-        <v>3.162385</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.66945900000000003</v>
-      </c>
-      <c r="F5" s="2">
-        <v>2.6294110000000002</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0.58426</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+      <c r="B6" s="13">
+        <v>0.18007400000000001</v>
+      </c>
+      <c r="C6" s="4">
+        <v>5.2528999999999999E-2</v>
+      </c>
+      <c r="D6" s="11">
+        <v>2.927076</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.59327600000000003</v>
+      </c>
+      <c r="F6" s="11">
+        <v>2.406755</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0.46395399999999998</v>
+      </c>
+      <c r="H6" s="9">
+        <f t="shared" si="0"/>
+        <v>5.5139049999999994</v>
+      </c>
+      <c r="I6" s="5">
+        <f t="shared" si="1"/>
+        <v>3.265816150260116E-2</v>
+      </c>
+      <c r="J6" s="5">
+        <f t="shared" si="2"/>
+        <v>0.53085354209040603</v>
+      </c>
+      <c r="K6" s="5">
+        <f t="shared" si="3"/>
+        <v>0.43648829640699294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
-        <v>0.20158499999999999</v>
-      </c>
-      <c r="C6" s="2">
-        <v>8.7070999999999996E-2</v>
-      </c>
-      <c r="D6" s="2">
-        <v>4.8000000000000001E-4</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1.2800000000000001E-3</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1.6919999999999999E-3</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1.5449999999999999E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="B7" s="13">
+        <v>0.158967</v>
+      </c>
+      <c r="C7" s="4">
+        <v>3.0669999999999999E-2</v>
+      </c>
+      <c r="D7" s="11">
+        <v>3.4900000000000003E-4</v>
+      </c>
+      <c r="E7" s="4">
+        <v>6.6600000000000003E-4</v>
+      </c>
+      <c r="F7" s="11">
+        <v>1.354E-3</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1.74E-4</v>
+      </c>
+      <c r="H7" s="9">
+        <f t="shared" si="0"/>
+        <v>0.16066999999999998</v>
+      </c>
+      <c r="I7" s="5">
+        <f t="shared" si="1"/>
+        <v>0.9894006348416009</v>
+      </c>
+      <c r="J7" s="5">
+        <f t="shared" si="2"/>
+        <v>2.1721541046866252E-3</v>
+      </c>
+      <c r="K7" s="5">
+        <f t="shared" si="3"/>
+        <v>8.4272110537125799E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
-        <v>1.2000379999999999</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0.41001500000000002</v>
-      </c>
-      <c r="D7" s="2">
-        <v>0.66286800000000001</v>
-      </c>
-      <c r="E7" s="2">
-        <v>0.238708</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0.40106399999999998</v>
-      </c>
-      <c r="G7" s="2">
-        <v>0.135742</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="B8" s="13">
+        <v>1.0001040000000001</v>
+      </c>
+      <c r="C8" s="4">
+        <v>0.201547</v>
+      </c>
+      <c r="D8" s="11">
+        <v>0.55108999999999997</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.136485</v>
+      </c>
+      <c r="F8" s="11">
+        <v>0.32652900000000001</v>
+      </c>
+      <c r="G8" s="4">
+        <v>8.5014999999999993E-2</v>
+      </c>
+      <c r="H8" s="9">
+        <f t="shared" si="0"/>
+        <v>1.8777230000000003</v>
+      </c>
+      <c r="I8" s="5">
+        <f t="shared" si="1"/>
+        <v>0.53261530055285045</v>
+      </c>
+      <c r="J8" s="5">
+        <f t="shared" si="2"/>
+        <v>0.2934884431835792</v>
+      </c>
+      <c r="K8" s="5">
+        <f t="shared" si="3"/>
+        <v>0.17389625626357028</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="2">
-        <v>4.5304440000000001</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1.1107629999999999</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1.321518</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.35930299999999998</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1.0252000000000001E-2</v>
-      </c>
-      <c r="G8" s="2">
-        <v>5.5370000000000003E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+      <c r="B9" s="13">
+        <v>4.1733029999999998</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.85814000000000001</v>
+      </c>
+      <c r="D9" s="11">
+        <v>1.31497</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.30520599999999998</v>
+      </c>
+      <c r="F9" s="11">
+        <v>9.3240000000000007E-3</v>
+      </c>
+      <c r="G9" s="4">
+        <v>3.803E-3</v>
+      </c>
+      <c r="H9" s="9">
+        <f t="shared" si="0"/>
+        <v>5.4975969999999998</v>
+      </c>
+      <c r="I9" s="5">
+        <f t="shared" si="1"/>
+        <v>0.75911402745599577</v>
+      </c>
+      <c r="J9" s="5">
+        <f t="shared" si="2"/>
+        <v>0.23918995881291408</v>
+      </c>
+      <c r="K9" s="5">
+        <f t="shared" si="3"/>
+        <v>1.6960137310901473E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="2">
-        <v>0.180058</v>
-      </c>
-      <c r="C9" s="2">
-        <v>5.9840999999999998E-2</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1.4205000000000001E-2</v>
-      </c>
-      <c r="E9" s="2">
-        <v>7.2909999999999997E-3</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.53528100000000001</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0.13026699999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+      <c r="B10" s="13">
+        <v>0.16120200000000001</v>
+      </c>
+      <c r="C10" s="4">
+        <v>9.5376000000000002E-2</v>
+      </c>
+      <c r="D10" s="11">
+        <v>1.3526E-2</v>
+      </c>
+      <c r="E10" s="4">
+        <v>3.954E-3</v>
+      </c>
+      <c r="F10" s="11">
+        <v>0.52793400000000001</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.106699</v>
+      </c>
+      <c r="H10" s="9">
+        <f t="shared" si="0"/>
+        <v>0.70266200000000001</v>
+      </c>
+      <c r="I10" s="5">
+        <f t="shared" si="1"/>
+        <v>0.22941613464226043</v>
+      </c>
+      <c r="J10" s="5">
+        <f t="shared" si="2"/>
+        <v>1.9249653460696608E-2</v>
+      </c>
+      <c r="K10" s="5">
+        <f t="shared" si="3"/>
+        <v>0.75133421189704297</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="2">
-        <v>0.15038899999999999</v>
-      </c>
-      <c r="C10" s="2">
-        <v>7.2169999999999998E-2</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.34794000000000003</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.124418</v>
-      </c>
-      <c r="F10" s="2">
-        <v>8.5516999999999996E-2</v>
-      </c>
-      <c r="G10" s="2">
-        <v>3.1767999999999998E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="B11" s="13">
+        <v>0.124458</v>
+      </c>
+      <c r="C11" s="4">
+        <v>3.9844999999999998E-2</v>
+      </c>
+      <c r="D11" s="11">
+        <v>0.29507299999999997</v>
+      </c>
+      <c r="E11" s="4">
+        <v>7.5705999999999996E-2</v>
+      </c>
+      <c r="F11" s="11">
+        <v>7.5289999999999996E-2</v>
+      </c>
+      <c r="G11" s="4">
+        <v>2.1406999999999999E-2</v>
+      </c>
+      <c r="H11" s="9">
+        <f t="shared" si="0"/>
+        <v>0.49482099999999996</v>
+      </c>
+      <c r="I11" s="5">
+        <f t="shared" si="1"/>
+        <v>0.25152125718189006</v>
+      </c>
+      <c r="J11" s="5">
+        <f t="shared" si="2"/>
+        <v>0.59632271063677578</v>
+      </c>
+      <c r="K11" s="5">
+        <f t="shared" si="3"/>
+        <v>0.15215603218133428</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="2">
-        <v>8.6862999999999996E-2</v>
-      </c>
-      <c r="C11" s="2">
-        <v>4.8404999999999997E-2</v>
-      </c>
-      <c r="D11" s="2">
-        <v>8.5899999999999995E-4</v>
-      </c>
-      <c r="E11" s="2">
-        <v>1.6180000000000001E-3</v>
-      </c>
-      <c r="F11" s="2">
-        <v>1.709E-3</v>
-      </c>
-      <c r="G11" s="2">
+      <c r="B12" s="13">
+        <v>6.3532000000000005E-2</v>
+      </c>
+      <c r="C12" s="4">
+        <v>1.9736E-2</v>
+      </c>
+      <c r="D12" s="11">
+        <v>7.0699999999999995E-4</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1.6659999999999999E-3</v>
+      </c>
+      <c r="F12" s="11">
+        <v>1.15E-3</v>
+      </c>
+      <c r="G12" s="4">
+        <v>1.2340000000000001E-3</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" si="0"/>
+        <v>6.5389000000000003E-2</v>
+      </c>
+      <c r="I12" s="5">
+        <f t="shared" si="1"/>
+        <v>0.97160072795118446</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" si="2"/>
+        <v>1.0812216121977702E-2</v>
+      </c>
+      <c r="K12" s="5">
+        <f t="shared" si="3"/>
+        <v>1.7587055926837847E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="13">
+        <v>0.164463</v>
+      </c>
+      <c r="C13" s="4">
+        <v>4.4547000000000003E-2</v>
+      </c>
+      <c r="D13" s="11">
+        <v>9.665934</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1.1707559999999999</v>
+      </c>
+      <c r="F13" s="11">
+        <v>22.647563000000002</v>
+      </c>
+      <c r="G13" s="4">
+        <v>3.1570689999999999</v>
+      </c>
+      <c r="H13" s="9">
+        <f t="shared" si="0"/>
+        <v>32.477960000000003</v>
+      </c>
+      <c r="I13" s="5">
+        <f t="shared" si="1"/>
+        <v>5.063834058543085E-3</v>
+      </c>
+      <c r="J13" s="5">
+        <f t="shared" si="2"/>
+        <v>0.29761518272699389</v>
+      </c>
+      <c r="K13" s="5">
+        <f t="shared" si="3"/>
+        <v>0.69732098321446301</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="13">
+        <v>0.100412</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2.3973999999999999E-2</v>
+      </c>
+      <c r="D14" s="11">
         <v>2.836E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.21859700000000001</v>
-      </c>
-      <c r="C12" s="2">
-        <v>7.5594999999999996E-2</v>
-      </c>
-      <c r="D12" s="2">
-        <v>9.8602070000000008</v>
-      </c>
-      <c r="E12" s="2">
-        <v>1.9718659999999999</v>
-      </c>
-      <c r="F12" s="2">
-        <v>22.078710999999998</v>
-      </c>
-      <c r="G12" s="2">
-        <v>2.6741980000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2">
-        <v>9.9238999999999994E-2</v>
-      </c>
-      <c r="C13" s="2">
-        <v>3.0304999999999999E-2</v>
-      </c>
-      <c r="D13" s="2">
-        <v>2.9710000000000001E-3</v>
-      </c>
-      <c r="E13" s="2">
-        <v>2.7169999999999998E-3</v>
-      </c>
-      <c r="F13" s="2">
-        <v>3.3400000000000001E-3</v>
-      </c>
-      <c r="G13" s="2">
-        <v>1.6720000000000001E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+      <c r="E14" s="4">
+        <v>2.1879999999999998E-3</v>
+      </c>
+      <c r="F14" s="11">
+        <v>3.7650000000000001E-3</v>
+      </c>
+      <c r="G14" s="4">
+        <v>3.1020000000000002E-3</v>
+      </c>
+      <c r="H14" s="9">
+        <f t="shared" si="0"/>
+        <v>0.10701300000000001</v>
+      </c>
+      <c r="I14" s="5">
+        <f t="shared" si="1"/>
+        <v>0.93831590554418609</v>
+      </c>
+      <c r="J14" s="5">
+        <f t="shared" si="2"/>
+        <v>2.6501453094483846E-2</v>
+      </c>
+      <c r="K14" s="5">
+        <f t="shared" si="3"/>
+        <v>3.5182641361329932E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="2">
-        <v>6.2486E-2</v>
-      </c>
-      <c r="C14" s="2">
-        <v>2.2298999999999999E-2</v>
-      </c>
-      <c r="D14" s="2">
-        <v>3.68E-4</v>
-      </c>
-      <c r="E14" s="2">
-        <v>6.0999999999999999E-5</v>
-      </c>
-      <c r="F14" s="2">
-        <v>7.1500000000000003E-4</v>
-      </c>
-      <c r="G14" s="2">
-        <v>8.2000000000000001E-5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+      <c r="B15" s="13">
+        <v>6.0907999999999997E-2</v>
+      </c>
+      <c r="C15" s="4">
+        <v>1.8241E-2</v>
+      </c>
+      <c r="D15" s="11">
+        <v>3.6600000000000001E-4</v>
+      </c>
+      <c r="E15" s="4">
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="F15" s="11">
+        <v>7.9900000000000001E-4</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1.665E-3</v>
+      </c>
+      <c r="H15" s="9">
+        <f t="shared" si="0"/>
+        <v>6.2072999999999996E-2</v>
+      </c>
+      <c r="I15" s="5">
+        <f t="shared" si="1"/>
+        <v>0.98123177549014873</v>
+      </c>
+      <c r="J15" s="5">
+        <f t="shared" si="2"/>
+        <v>5.8962834082451308E-3</v>
+      </c>
+      <c r="K15" s="5">
+        <f t="shared" si="3"/>
+        <v>1.2871941101606174E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="2">
-        <v>0.15820000000000001</v>
-      </c>
-      <c r="C15" s="2">
-        <v>4.8443E-2</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.59872899999999996</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.13619200000000001</v>
-      </c>
-      <c r="F15" s="2">
-        <v>11.479832999999999</v>
-      </c>
-      <c r="G15" s="2">
-        <v>1.8168800000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+      <c r="B16" s="13">
+        <v>0.16551199999999999</v>
+      </c>
+      <c r="C16" s="4">
+        <v>4.2792999999999998E-2</v>
+      </c>
+      <c r="D16" s="11">
+        <v>0.58871200000000001</v>
+      </c>
+      <c r="E16" s="4">
+        <v>0.159972</v>
+      </c>
+      <c r="F16" s="11">
+        <v>11.132872000000001</v>
+      </c>
+      <c r="G16" s="4">
+        <v>1.2454320000000001</v>
+      </c>
+      <c r="H16" s="9">
+        <f t="shared" si="0"/>
+        <v>11.887096000000001</v>
+      </c>
+      <c r="I16" s="5">
+        <f t="shared" si="1"/>
+        <v>1.392366983492015E-2</v>
+      </c>
+      <c r="J16" s="5">
+        <f t="shared" si="2"/>
+        <v>4.9525300376138962E-2</v>
+      </c>
+      <c r="K16" s="5">
+        <f t="shared" si="3"/>
+        <v>0.93655102978894078</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="2">
-        <v>0.22489999999999999</v>
-      </c>
-      <c r="C16" s="2">
-        <v>4.0258000000000002E-2</v>
-      </c>
-      <c r="D16" s="2">
-        <v>5.4749999999999998E-3</v>
-      </c>
-      <c r="E16" s="2">
-        <v>3.6999999999999999E-4</v>
-      </c>
-      <c r="F16" s="2">
-        <v>890.40279999999996</v>
-      </c>
-      <c r="G16" s="2">
-        <v>25.593371000000001</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+      <c r="B17" s="13">
+        <v>0.20652000000000001</v>
+      </c>
+      <c r="C17" s="4">
+        <v>5.5454000000000003E-2</v>
+      </c>
+      <c r="D17" s="11">
+        <v>6.5399999999999998E-3</v>
+      </c>
+      <c r="E17" s="4">
+        <v>3.2929999999999999E-3</v>
+      </c>
+      <c r="F17" s="11">
+        <v>865.05989999999997</v>
+      </c>
+      <c r="G17" s="4">
+        <v>16.886956999999999</v>
+      </c>
+      <c r="H17" s="9">
+        <f t="shared" si="0"/>
+        <v>865.27296000000001</v>
+      </c>
+      <c r="I17" s="5">
+        <f t="shared" si="1"/>
+        <v>2.3867612828210882E-4</v>
+      </c>
+      <c r="J17" s="5">
+        <f t="shared" si="2"/>
+        <v>7.5583085365339507E-6</v>
+      </c>
+      <c r="K17" s="5">
+        <f t="shared" si="3"/>
+        <v>0.9997537655631813</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="2">
-        <v>0.473383</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0.143709</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0.179065</v>
-      </c>
-      <c r="E17" s="2">
-        <v>5.416E-2</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0.49242999999999998</v>
-      </c>
-      <c r="G17" s="2">
-        <v>0.143015</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+      <c r="B18" s="13">
+        <v>0.44292999999999999</v>
+      </c>
+      <c r="C18" s="4">
+        <v>0.101872</v>
+      </c>
+      <c r="D18" s="11">
+        <v>0.16650699999999999</v>
+      </c>
+      <c r="E18" s="4">
+        <v>3.2071000000000002E-2</v>
+      </c>
+      <c r="F18" s="11">
+        <v>0.45431300000000002</v>
+      </c>
+      <c r="G18" s="4">
+        <v>8.3112000000000005E-2</v>
+      </c>
+      <c r="H18" s="9">
+        <f t="shared" si="0"/>
+        <v>1.06375</v>
+      </c>
+      <c r="I18" s="5">
+        <f t="shared" si="1"/>
+        <v>0.41638542890716806</v>
+      </c>
+      <c r="J18" s="5">
+        <f t="shared" si="2"/>
+        <v>0.15652831962397179</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" si="3"/>
+        <v>0.4270862514688602</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+      <c r="B19" s="13">
+        <v>0.12964899999999999</v>
+      </c>
+      <c r="C19" s="4">
+        <v>4.0571999999999997E-2</v>
+      </c>
+      <c r="D19" s="11">
+        <v>0.382911</v>
+      </c>
+      <c r="E19" s="4">
+        <v>8.8095000000000007E-2</v>
+      </c>
+      <c r="F19" s="11">
+        <v>10.257724</v>
+      </c>
+      <c r="G19" s="4">
+        <v>1.290351</v>
+      </c>
+      <c r="H19" s="9">
+        <f t="shared" si="0"/>
+        <v>10.770284</v>
+      </c>
+      <c r="I19" s="5">
+        <f t="shared" ref="I19" si="4">+B19/$H19</f>
+        <v>1.2037658431291133E-2</v>
+      </c>
+      <c r="J19" s="5">
+        <f t="shared" ref="J19" si="5">+D19/H19</f>
+        <v>3.5552544389730115E-2</v>
+      </c>
+      <c r="K19" s="5">
+        <f t="shared" ref="K19" si="6">+F19/H19</f>
+        <v>0.95240979717897867</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+      <c r="B20" s="13"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="9">
+        <f>+B20+D20+F20</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="3">
+      <c r="B21" s="13"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="B22" s="13"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+      <c r="B23" s="13"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5"/>
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+      <c r="B24" s="13"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5"/>
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="3">
+      <c r="B25" s="13"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+      <c r="K25" s="5"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
         <v>24</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="3">
+      <c r="B26" s="13"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
+      <c r="K26" s="5"/>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="15">
         <v>25</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="3"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="B27" s="17"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="3"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+      <c r="K28" s="6"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="2">
-        <f>+AVERAGE(B2:B26)</f>
-        <v>0.57010462500000003</v>
-      </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2">
-        <f>+AVERAGE(D2:D26)</f>
-        <v>1.0328058125000001</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2">
-        <f>+AVERAGE(F2:F26)</f>
-        <v>58.083734874999998</v>
-      </c>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+      <c r="B29" s="13">
+        <f>+AVERAGE(B3:B27)</f>
+        <v>0.49237223529411778</v>
+      </c>
+      <c r="C29" s="4"/>
+      <c r="D29" s="11">
+        <f>+AVERAGE(D3:D27)</f>
+        <v>0.95913447058823498</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="11">
+        <f>+AVERAGE(F3:F27)</f>
+        <v>53.768110294117648</v>
+      </c>
+      <c r="G29" s="4"/>
+      <c r="H29" s="9">
+        <f>+SUM(H3:H27)</f>
+        <v>938.73348899999996</v>
+      </c>
+      <c r="I29" s="7">
+        <f>+AVERAGE(I3:I27)</f>
+        <v>0.43244683811361806</v>
+      </c>
+      <c r="J29" s="7">
+        <f t="shared" ref="J29:K29" si="7">+AVERAGE(J3:J27)</f>
+        <v>0.17809107826287565</v>
+      </c>
+      <c r="K29" s="7">
+        <f t="shared" si="7"/>
+        <v>0.38946208362350621</v>
+      </c>
+      <c r="L29" s="2"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B29" s="2">
-        <f>+MEDIAN(B2:B26)</f>
-        <v>0.19082149999999998</v>
-      </c>
-      <c r="D29" s="2">
-        <f>+MEDIAN(D2:D26)</f>
-        <v>0.10320499999999999</v>
-      </c>
-      <c r="F29" s="2">
-        <f>+MEDIAN(F2:F26)</f>
-        <v>0.26024349999999996</v>
-      </c>
+      <c r="B30" s="13">
+        <f>+MEDIAN(B3:B27)</f>
+        <v>0.16120200000000001</v>
+      </c>
+      <c r="C30" s="8"/>
+      <c r="D30" s="11">
+        <f>+MEDIAN(D3:D27)</f>
+        <v>0.16650699999999999</v>
+      </c>
+      <c r="E30" s="8"/>
+      <c r="F30" s="11">
+        <f>+MEDIAN(F3:F27)</f>
+        <v>0.32652900000000001</v>
+      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
+  <mergeCells count="5">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="I1:K1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B2:B26">
+  <conditionalFormatting sqref="B3:B27">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="greaterThan">
+      <formula>$B$29</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="lessThan">
+      <formula>$B$29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D3:D27">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="greaterThan">
+      <formula>$D$29</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="lessThan">
+      <formula>$D$29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F3:F27">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
-      <formula>$B$28</formula>
+      <formula>$F$29</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThan">
-      <formula>$B$28</formula>
+      <formula>$F$29</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D26">
+  <conditionalFormatting sqref="I3:I27">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
-      <formula>$D$28</formula>
+      <formula>$I$29</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="4" operator="lessThan">
-      <formula>$D$28</formula>
+      <formula>$I$29</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F26">
+  <conditionalFormatting sqref="J3:K27">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
-      <formula>$F$28</formula>
+      <formula>$K$29</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
-      <formula>$F$28</formula>
+      <formula>$K$29</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2908,6 +3675,833 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C255480-31BF-4ACB-A6C3-15B60FC32034}">
+  <dimension ref="A1:N17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>72594</v>
+      </c>
+      <c r="C1">
+        <v>44951</v>
+      </c>
+      <c r="D1">
+        <v>16238</v>
+      </c>
+      <c r="E1">
+        <v>2778</v>
+      </c>
+      <c r="F1">
+        <v>1039283</v>
+      </c>
+      <c r="G1">
+        <v>98209</v>
+      </c>
+      <c r="I1">
+        <f>+B1/1000000</f>
+        <v>7.2594000000000006E-2</v>
+      </c>
+      <c r="J1">
+        <f t="shared" ref="J1:N16" si="0">+C1/1000000</f>
+        <v>4.4950999999999998E-2</v>
+      </c>
+      <c r="K1">
+        <f t="shared" si="0"/>
+        <v>1.6237999999999999E-2</v>
+      </c>
+      <c r="L1">
+        <f t="shared" si="0"/>
+        <v>2.7780000000000001E-3</v>
+      </c>
+      <c r="M1">
+        <f t="shared" si="0"/>
+        <v>1.039283</v>
+      </c>
+      <c r="N1">
+        <f t="shared" si="0"/>
+        <v>9.8209000000000005E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>129563</v>
+      </c>
+      <c r="C2">
+        <v>26047</v>
+      </c>
+      <c r="D2">
+        <v>346487</v>
+      </c>
+      <c r="E2">
+        <v>63133</v>
+      </c>
+      <c r="F2">
+        <v>323</v>
+      </c>
+      <c r="G2">
+        <v>48</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:I17" si="1">+B2/1000000</f>
+        <v>0.12956300000000001</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="0"/>
+        <v>2.6047000000000001E-2</v>
+      </c>
+      <c r="K2">
+        <f t="shared" si="0"/>
+        <v>0.34648699999999999</v>
+      </c>
+      <c r="L2">
+        <f t="shared" si="0"/>
+        <v>6.3132999999999995E-2</v>
+      </c>
+      <c r="M2">
+        <f t="shared" si="0"/>
+        <v>3.2299999999999999E-4</v>
+      </c>
+      <c r="N2">
+        <f t="shared" si="0"/>
+        <v>4.8000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1036137</v>
+      </c>
+      <c r="C3">
+        <v>138641</v>
+      </c>
+      <c r="D3">
+        <v>25964</v>
+      </c>
+      <c r="E3">
+        <v>5420</v>
+      </c>
+      <c r="F3">
+        <v>112997</v>
+      </c>
+      <c r="G3">
+        <v>14442</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="1"/>
+        <v>1.0361370000000001</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>0.13864099999999999</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>2.5964000000000001E-2</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>5.4200000000000003E-3</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="0"/>
+        <v>0.112997</v>
+      </c>
+      <c r="N3">
+        <f t="shared" si="0"/>
+        <v>1.4442E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>180074</v>
+      </c>
+      <c r="C4">
+        <v>52529</v>
+      </c>
+      <c r="D4">
+        <v>2927076</v>
+      </c>
+      <c r="E4">
+        <v>593276</v>
+      </c>
+      <c r="F4">
+        <v>2406755</v>
+      </c>
+      <c r="G4">
+        <v>463954</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>0.18007400000000001</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>5.2528999999999999E-2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>2.927076</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>0.59327600000000003</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>2.406755</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="0"/>
+        <v>0.46395399999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>158967</v>
+      </c>
+      <c r="C5">
+        <v>30670</v>
+      </c>
+      <c r="D5">
+        <v>349</v>
+      </c>
+      <c r="E5">
+        <v>666</v>
+      </c>
+      <c r="F5">
+        <v>1354</v>
+      </c>
+      <c r="G5">
+        <v>174</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>0.158967</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>3.0669999999999999E-2</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>3.4900000000000003E-4</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>6.6600000000000003E-4</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="0"/>
+        <v>1.354E-3</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="0"/>
+        <v>1.74E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>1000104</v>
+      </c>
+      <c r="C6">
+        <v>201547</v>
+      </c>
+      <c r="D6">
+        <v>551090</v>
+      </c>
+      <c r="E6">
+        <v>136485</v>
+      </c>
+      <c r="F6">
+        <v>326529</v>
+      </c>
+      <c r="G6">
+        <v>85015</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>1.0001040000000001</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>0.201547</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>0.55108999999999997</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>0.136485</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="0"/>
+        <v>0.32652900000000001</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="0"/>
+        <v>8.5014999999999993E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>4173303</v>
+      </c>
+      <c r="C7">
+        <v>858140</v>
+      </c>
+      <c r="D7">
+        <v>1314970</v>
+      </c>
+      <c r="E7">
+        <v>305206</v>
+      </c>
+      <c r="F7">
+        <v>9324</v>
+      </c>
+      <c r="G7">
+        <v>3803</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>4.1733029999999998</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>0.85814000000000001</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>1.31497</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>0.30520599999999998</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>9.3240000000000007E-3</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="0"/>
+        <v>3.803E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>161202</v>
+      </c>
+      <c r="C8">
+        <v>95376</v>
+      </c>
+      <c r="D8">
+        <v>13526</v>
+      </c>
+      <c r="E8">
+        <v>3954</v>
+      </c>
+      <c r="F8">
+        <v>527934</v>
+      </c>
+      <c r="G8">
+        <v>106699</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>0.16120200000000001</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>9.5376000000000002E-2</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>1.3526E-2</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>3.954E-3</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="0"/>
+        <v>0.52793400000000001</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="0"/>
+        <v>0.106699</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>124458</v>
+      </c>
+      <c r="C9">
+        <v>39845</v>
+      </c>
+      <c r="D9">
+        <v>295073</v>
+      </c>
+      <c r="E9">
+        <v>75706</v>
+      </c>
+      <c r="F9">
+        <v>75290</v>
+      </c>
+      <c r="G9">
+        <v>21407</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0.124458</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>3.9844999999999998E-2</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>0.29507299999999997</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>7.5705999999999996E-2</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>7.5289999999999996E-2</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="0"/>
+        <v>2.1406999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>63532</v>
+      </c>
+      <c r="C10">
+        <v>19736</v>
+      </c>
+      <c r="D10">
+        <v>707</v>
+      </c>
+      <c r="E10">
+        <v>1666</v>
+      </c>
+      <c r="F10">
+        <v>1150</v>
+      </c>
+      <c r="G10">
+        <v>1234</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>6.3532000000000005E-2</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>1.9736E-2</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>7.0699999999999995E-4</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>1.6659999999999999E-3</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="0"/>
+        <v>1.15E-3</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="0"/>
+        <v>1.2340000000000001E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>164463</v>
+      </c>
+      <c r="C11">
+        <v>44547</v>
+      </c>
+      <c r="D11">
+        <v>9665934</v>
+      </c>
+      <c r="E11">
+        <v>1170756</v>
+      </c>
+      <c r="F11">
+        <v>22647563</v>
+      </c>
+      <c r="G11">
+        <v>3157069</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0.164463</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>4.4547000000000003E-2</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>9.665934</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>1.1707559999999999</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>22.647563000000002</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="0"/>
+        <v>3.1570689999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>100412</v>
+      </c>
+      <c r="C12">
+        <v>23974</v>
+      </c>
+      <c r="D12">
+        <v>2836</v>
+      </c>
+      <c r="E12">
+        <v>2188</v>
+      </c>
+      <c r="F12">
+        <v>3765</v>
+      </c>
+      <c r="G12">
+        <v>3102</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>0.100412</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>2.3973999999999999E-2</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>2.836E-3</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>2.1879999999999998E-3</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="0"/>
+        <v>3.7650000000000001E-3</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="0"/>
+        <v>3.1020000000000002E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>60908</v>
+      </c>
+      <c r="C13">
+        <v>18241</v>
+      </c>
+      <c r="D13">
+        <v>366</v>
+      </c>
+      <c r="E13">
+        <v>60</v>
+      </c>
+      <c r="F13">
+        <v>799</v>
+      </c>
+      <c r="G13">
+        <v>1665</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>6.0907999999999997E-2</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>1.8241E-2</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>3.6600000000000001E-4</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>6.0000000000000002E-5</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>7.9900000000000001E-4</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="0"/>
+        <v>1.665E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>165512</v>
+      </c>
+      <c r="C14">
+        <v>42793</v>
+      </c>
+      <c r="D14">
+        <v>588712</v>
+      </c>
+      <c r="E14">
+        <v>159972</v>
+      </c>
+      <c r="F14">
+        <v>11132872</v>
+      </c>
+      <c r="G14">
+        <v>1245432</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>0.16551199999999999</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>4.2792999999999998E-2</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>0.58871200000000001</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>0.159972</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="0"/>
+        <v>11.132872000000001</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="0"/>
+        <v>1.2454320000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>206520</v>
+      </c>
+      <c r="C15">
+        <v>55454</v>
+      </c>
+      <c r="D15">
+        <v>6540</v>
+      </c>
+      <c r="E15">
+        <v>3293</v>
+      </c>
+      <c r="F15">
+        <v>865059900</v>
+      </c>
+      <c r="G15">
+        <v>16886957</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>0.20652000000000001</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>5.5454000000000003E-2</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>6.5399999999999998E-3</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>3.2929999999999999E-3</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>865.05989999999997</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>16.886956999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>442930</v>
+      </c>
+      <c r="C16">
+        <v>101872</v>
+      </c>
+      <c r="D16">
+        <v>166507</v>
+      </c>
+      <c r="E16">
+        <v>32071</v>
+      </c>
+      <c r="F16">
+        <v>454313</v>
+      </c>
+      <c r="G16">
+        <v>83112</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>0.44292999999999999</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>0.101872</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="0"/>
+        <v>0.16650699999999999</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>3.2071000000000002E-2</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="0"/>
+        <v>0.45431300000000002</v>
+      </c>
+      <c r="N16">
+        <f t="shared" si="0"/>
+        <v>8.3112000000000005E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>129649</v>
+      </c>
+      <c r="C17">
+        <v>40572</v>
+      </c>
+      <c r="D17">
+        <v>382911</v>
+      </c>
+      <c r="E17">
+        <v>88095</v>
+      </c>
+      <c r="F17">
+        <v>10257724</v>
+      </c>
+      <c r="G17">
+        <v>1290351</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>0.12964899999999999</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ref="J17" si="2">+C17/1000000</f>
+        <v>4.0571999999999997E-2</v>
+      </c>
+      <c r="K17">
+        <f t="shared" ref="K17" si="3">+D17/1000000</f>
+        <v>0.382911</v>
+      </c>
+      <c r="L17">
+        <f t="shared" ref="L17" si="4">+E17/1000000</f>
+        <v>8.8095000000000007E-2</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ref="M17" si="5">+F17/1000000</f>
+        <v>10.257724</v>
+      </c>
+      <c r="N17">
+        <f t="shared" ref="N17" si="6">+G17/1000000</f>
+        <v>1.290351</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21C7AF5-2DCC-4E61-8CEE-E5E160A12B00}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E000E53-3210-4B5E-B4E9-4D5038408630}">
   <dimension ref="A1:M1"/>
   <sheetViews>
@@ -2966,7 +4560,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{654FFB1D-6211-4980-B041-A90B27A14703}">
   <dimension ref="A1:M1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Updated analysis after day 18
</commit_message>
<xml_diff>
--- a/2020/analysis/execution times.xlsx
+++ b/2020/analysis/execution times.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\arno\git\AdventOfCode\2020\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C30D81A-8E3E-447A-B5E8-0EE6957DE5D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6372E6F-4EA8-45E1-A3C1-6901847A1245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{23AEBC82-DD3C-489D-BC2D-D322F6541D25}"/>
   </bookViews>
   <sheets>
     <sheet name="analysis" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -561,58 +562,79 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="25"/>
                   <c:pt idx="0">
-                    <c:v>3.7600000000000001E-2</c:v>
+                    <c:v>0.46389999999999998</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.7900000000000001E-2</c:v>
+                    <c:v>0.44629999999999997</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.15659999999999999</c:v>
+                    <c:v>0.46100000000000002</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.24E-2</c:v>
+                    <c:v>0.45650000000000002</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.7E-2</c:v>
+                    <c:v>0.38529999999999998</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.16159999999999999</c:v>
+                    <c:v>0.45850000000000002</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.90410000000000001</c:v>
+                    <c:v>1.3262</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>4.2799999999999998E-2</c:v>
+                    <c:v>0.46379999999999999</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>5.0500000000000003E-2</c:v>
+                    <c:v>0.40039999999999998</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>2.3E-2</c:v>
+                    <c:v>0.2301</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>6.0699999999999997E-2</c:v>
+                    <c:v>0.74770000000000003</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>2.1700000000000001E-2</c:v>
+                    <c:v>0.4773</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>1.6E-2</c:v>
+                    <c:v>0.2354</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>4.4900000000000002E-2</c:v>
+                    <c:v>1.1701999999999999</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>4.7500000000000001E-2</c:v>
+                    <c:v>1.4416</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>0.81499999999999995</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>2.9700000000000001E-2</c:v>
+                    <c:v>0.69399999999999995</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>1.72E-2</c:v>
+                    <c:v>3.3799999999999997E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.5800000000000002E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>1.9900000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>2.1999999999999999E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>2.6100000000000002E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>2.01E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>2.9600000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>1.9800000000000002E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -624,58 +646,79 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="25"/>
                   <c:pt idx="0">
-                    <c:v>3.7600000000000001E-2</c:v>
+                    <c:v>0.46389999999999998</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>2.7900000000000001E-2</c:v>
+                    <c:v>0.44629999999999997</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.15659999999999999</c:v>
+                    <c:v>0.46100000000000002</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>4.24E-2</c:v>
+                    <c:v>0.45650000000000002</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>2.7E-2</c:v>
+                    <c:v>0.38529999999999998</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>0.16159999999999999</c:v>
+                    <c:v>0.45850000000000002</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.90410000000000001</c:v>
+                    <c:v>1.3262</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>4.2799999999999998E-2</c:v>
+                    <c:v>0.46379999999999999</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>5.0500000000000003E-2</c:v>
+                    <c:v>0.40039999999999998</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>2.3E-2</c:v>
+                    <c:v>0.2301</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>6.0699999999999997E-2</c:v>
+                    <c:v>0.74770000000000003</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>2.1700000000000001E-2</c:v>
+                    <c:v>0.4773</c:v>
                   </c:pt>
                   <c:pt idx="12">
-                    <c:v>1.6E-2</c:v>
+                    <c:v>0.2354</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>4.4900000000000002E-2</c:v>
+                    <c:v>1.1701999999999999</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>4.7500000000000001E-2</c:v>
+                    <c:v>1.4416</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>7.0000000000000007E-2</c:v>
+                    <c:v>0.81499999999999995</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>2.9700000000000001E-2</c:v>
+                    <c:v>0.69399999999999995</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>1.72E-2</c:v>
+                    <c:v>3.3799999999999997E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.5800000000000002E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>1.9900000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>2.1999999999999999E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>2.6100000000000002E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>2.01E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>2.9600000000000001E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>1.9800000000000002E-2</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -764,58 +807,58 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>8.1199999999999994E-2</c:v>
+                  <c:v>9.2999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13350000000000001</c:v>
+                  <c:v>0.1623</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.0633999999999999</c:v>
+                  <c:v>1.0328999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.17960000000000001</c:v>
+                  <c:v>0.20080000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.15340000000000001</c:v>
+                  <c:v>0.17899999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0084</c:v>
+                  <c:v>1.0788</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.1924000000000001</c:v>
+                  <c:v>4.0505000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1449</c:v>
+                  <c:v>0.17879999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.13469999999999999</c:v>
+                  <c:v>0.1368</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6.1499999999999999E-2</c:v>
+                  <c:v>7.5300000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.15759999999999999</c:v>
+                  <c:v>0.22070000000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.10009999999999999</c:v>
+                  <c:v>0.1273</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.9400000000000001E-2</c:v>
+                  <c:v>7.1400000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.16819999999999999</c:v>
+                  <c:v>0.2868</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.1973</c:v>
+                  <c:v>0.65859999999999996</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.44519999999999998</c:v>
+                  <c:v>0.48859999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.16600000000000001</c:v>
+                  <c:v>0.2293</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.8099999999999997E-2</c:v>
+                  <c:v>0.1077</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -861,57 +904,78 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="25"/>
                   <c:pt idx="0">
-                    <c:v>5.7999999999999996E-3</c:v>
+                    <c:v>6.1000000000000004E-3</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.2200000000000003E-2</c:v>
+                    <c:v>5.1499999999999997E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.1000000000000004E-3</c:v>
+                    <c:v>4.8999999999999998E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.434</c:v>
+                    <c:v>0.51980000000000004</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>1.1999999999999999E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>9.4200000000000006E-2</c:v>
+                    <c:v>0.1802</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.29409999999999997</c:v>
+                    <c:v>0.2472</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>3.3999999999999998E-3</c:v>
+                    <c:v>7.0000000000000001E-3</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>8.9499999999999996E-2</c:v>
+                    <c:v>5.91E-2</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>1E-4</c:v>
+                    <c:v>1.2999999999999999E-3</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>1.88</c:v>
+                    <c:v>1.8113999999999999</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>1.2999999999999999E-3</c:v>
+                    <c:v>2.5000000000000001E-3</c:v>
                   </c:pt>
                   <c:pt idx="12">
                     <c:v>1E-4</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0.12540000000000001</c:v>
+                    <c:v>0.1353</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>5.9999999999999995E-4</c:v>
+                    <c:v>5.0000000000000001E-4</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>2.07E-2</c:v>
+                    <c:v>3.0800000000000001E-2</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>1.3631</c:v>
+                    <c:v>1.4458</c:v>
                   </c:pt>
                   <c:pt idx="17">
+                    <c:v>0.11459999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.1999999999999999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>1.2999999999999999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>1E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>1E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>1E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>2.9999999999999997E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
                     <c:v>1E-4</c:v>
                   </c:pt>
                 </c:numCache>
@@ -924,57 +988,78 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="25"/>
                   <c:pt idx="0">
-                    <c:v>5.7999999999999996E-3</c:v>
+                    <c:v>6.1000000000000004E-3</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>5.2200000000000003E-2</c:v>
+                    <c:v>5.1499999999999997E-2</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>7.1000000000000004E-3</c:v>
+                    <c:v>4.8999999999999998E-3</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>0.434</c:v>
+                    <c:v>0.51980000000000004</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>0</c:v>
+                    <c:v>1.1999999999999999E-3</c:v>
                   </c:pt>
                   <c:pt idx="5">
-                    <c:v>9.4200000000000006E-2</c:v>
+                    <c:v>0.1802</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v>0.29409999999999997</c:v>
+                    <c:v>0.2472</c:v>
                   </c:pt>
                   <c:pt idx="7">
-                    <c:v>3.3999999999999998E-3</c:v>
+                    <c:v>7.0000000000000001E-3</c:v>
                   </c:pt>
                   <c:pt idx="8">
-                    <c:v>8.9499999999999996E-2</c:v>
+                    <c:v>5.91E-2</c:v>
                   </c:pt>
                   <c:pt idx="9">
-                    <c:v>1E-4</c:v>
+                    <c:v>1.2999999999999999E-3</c:v>
                   </c:pt>
                   <c:pt idx="10">
-                    <c:v>1.88</c:v>
+                    <c:v>1.8113999999999999</c:v>
                   </c:pt>
                   <c:pt idx="11">
-                    <c:v>1.2999999999999999E-3</c:v>
+                    <c:v>2.5000000000000001E-3</c:v>
                   </c:pt>
                   <c:pt idx="12">
                     <c:v>1E-4</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>0.12540000000000001</c:v>
+                    <c:v>0.1353</c:v>
                   </c:pt>
                   <c:pt idx="14">
-                    <c:v>5.9999999999999995E-4</c:v>
+                    <c:v>5.0000000000000001E-4</c:v>
                   </c:pt>
                   <c:pt idx="15">
-                    <c:v>2.07E-2</c:v>
+                    <c:v>3.0800000000000001E-2</c:v>
                   </c:pt>
                   <c:pt idx="16">
-                    <c:v>1.3631</c:v>
+                    <c:v>1.4458</c:v>
                   </c:pt>
                   <c:pt idx="17">
+                    <c:v>0.11459999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.1999999999999999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>1.2999999999999999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>1E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>1E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>1E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>2.9999999999999997E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
                     <c:v>1E-4</c:v>
                   </c:pt>
                 </c:numCache>
@@ -1064,58 +1149,58 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1.72E-2</c:v>
+                  <c:v>1.6799999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.3584</c:v>
+                  <c:v>0.31909999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.69E-2</c:v>
+                  <c:v>2.5100000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.8792</c:v>
+                  <c:v>2.8708</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.9999999999999997E-4</c:v>
+                  <c:v>4.0000000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.55189999999999995</c:v>
+                  <c:v>0.58320000000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.3483000000000001</c:v>
+                  <c:v>0.98199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.29E-2</c:v>
+                  <c:v>1.41E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.30220000000000002</c:v>
+                  <c:v>0.27479999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.9999999999999995E-4</c:v>
+                  <c:v>6.9999999999999999E-4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.9281000000000006</c:v>
+                  <c:v>9.7632999999999992</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.5999999999999999E-3</c:v>
+                  <c:v>2.8E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>4.0000000000000002E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.60680000000000001</c:v>
+                  <c:v>0.61209999999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>5.4999999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.15770000000000001</c:v>
+                  <c:v>0.1474</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.4382000000000001</c:v>
+                  <c:v>7.3102999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.0000000000000002E-4</c:v>
+                  <c:v>0.60599999999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1161,57 +1246,78 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="25"/>
                   <c:pt idx="0">
-                    <c:v>0.12379999999999999</c:v>
+                    <c:v>0.1457</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>2.0000000000000001E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.8699999999999998E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.38</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.5000000000000001E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.122</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3.0999999999999999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.18720000000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1.2699999999999999E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>8.9999999999999998E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2.7014</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.5999999999999999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>1.4E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1.3191999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>22.526700000000002</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>9.3700000000000006E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>7.2497999999999996</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>0.12790000000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.2999999999999999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
                     <c:v>1E-4</c:v>
                   </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2.1100000000000001E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0.40620000000000001</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>1.6000000000000001E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>5.8500000000000003E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>3.3E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>0.1208</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>2.3900000000000001E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>1.4E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>3.4729000000000001</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>1.5E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="20">
+                    <c:v>4.0000000000000002E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
                     <c:v>1E-4</c:v>
                   </c:pt>
-                  <c:pt idx="13">
-                    <c:v>1.0256000000000001</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>19.710799999999999</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>4.9099999999999998E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>8.3059999999999992</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
+                  <c:pt idx="22">
+                    <c:v>6.9999999999999999E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>6.9999999999999999E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
                     <c:v>1E-4</c:v>
                   </c:pt>
                 </c:numCache>
@@ -1224,57 +1330,78 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="25"/>
                   <c:pt idx="0">
-                    <c:v>0.12379999999999999</c:v>
+                    <c:v>0.1457</c:v>
                   </c:pt>
                   <c:pt idx="1">
+                    <c:v>2.0000000000000001E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.8699999999999998E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.38</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.5000000000000001E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.122</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3.0999999999999999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.18720000000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>1.2699999999999999E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>8.9999999999999998E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>2.7014</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>2.5999999999999999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>1.4E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1.3191999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>22.526700000000002</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>9.3700000000000006E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>7.2497999999999996</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>0.12790000000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.2999999999999999E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
                     <c:v>1E-4</c:v>
                   </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2.1100000000000001E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0.40620000000000001</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>1.6000000000000001E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>5.8500000000000003E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>3.3E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>0.1208</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>2.3900000000000001E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>1.4E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>3.4729000000000001</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>1.5E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
+                  <c:pt idx="20">
+                    <c:v>4.0000000000000002E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
                     <c:v>1E-4</c:v>
                   </c:pt>
-                  <c:pt idx="13">
-                    <c:v>1.0256000000000001</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>19.710799999999999</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>4.9099999999999998E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>8.3059999999999992</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
+                  <c:pt idx="22">
+                    <c:v>6.9999999999999999E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>6.9999999999999999E-4</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
                     <c:v>1E-4</c:v>
                   </c:pt>
                 </c:numCache>
@@ -1364,58 +1491,58 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1.1207</c:v>
+                  <c:v>1.0470999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2.9999999999999997E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1171</c:v>
+                  <c:v>0.11210000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.3534999999999999</c:v>
+                  <c:v>2.3601999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2999999999999999E-3</c:v>
+                  <c:v>1.6000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.32269999999999999</c:v>
+                  <c:v>0.3619</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.1999999999999998E-3</c:v>
+                  <c:v>9.1000000000000004E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.52029999999999998</c:v>
+                  <c:v>0.56230000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.7600000000000002E-2</c:v>
+                  <c:v>5.7200000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1.1000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22.502700000000001</c:v>
+                  <c:v>22.0214</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.2000000000000002E-3</c:v>
+                  <c:v>3.5999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6.9999999999999999E-4</c:v>
+                  <c:v>8.0000000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.2263</c:v>
+                  <c:v>11.4954</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>876.95929999999998</c:v>
+                  <c:v>874.42840000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.4556</c:v>
+                  <c:v>0.46089999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>200.09180000000001</c:v>
+                  <c:v>206.36789999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.0000000000000002E-4</c:v>
+                  <c:v>0.60580000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2646,7 +2773,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC653439-E4E1-46BD-9CBD-A18AF82E67AB}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2708,38 +2837,38 @@
         <v>1</v>
       </c>
       <c r="B3" s="13">
-        <v>8.1199999999999994E-2</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="C3" s="4">
-        <v>3.7600000000000001E-2</v>
+        <v>0.46389999999999998</v>
       </c>
       <c r="D3" s="11">
-        <v>1.72E-2</v>
+        <v>1.6799999999999999E-2</v>
       </c>
       <c r="E3" s="4">
-        <v>5.7999999999999996E-3</v>
+        <v>6.1000000000000004E-3</v>
       </c>
       <c r="F3" s="11">
-        <v>1.1207</v>
+        <v>1.0470999999999999</v>
       </c>
       <c r="G3" s="4">
-        <v>0.12379999999999999</v>
+        <v>0.1457</v>
       </c>
       <c r="H3" s="9">
         <f>+B3+D3+F3</f>
-        <v>1.2191000000000001</v>
+        <v>1.1568999999999998</v>
       </c>
       <c r="I3" s="5">
         <f>+B3/$H3</f>
-        <v>6.660651300139446E-2</v>
+        <v>8.0387241766790574E-2</v>
       </c>
       <c r="J3" s="5">
         <f>+D3/H3</f>
-        <v>1.4108768763842178E-2</v>
+        <v>1.4521566254646038E-2</v>
       </c>
       <c r="K3" s="5">
         <f>+F3/H3</f>
-        <v>0.91928471823476332</v>
+        <v>0.90509119197856347</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -2747,38 +2876,38 @@
         <v>2</v>
       </c>
       <c r="B4" s="13">
-        <v>0.13350000000000001</v>
+        <v>0.1623</v>
       </c>
       <c r="C4" s="4">
-        <v>2.7900000000000001E-2</v>
+        <v>0.44629999999999997</v>
       </c>
       <c r="D4" s="11">
-        <v>0.3584</v>
+        <v>0.31909999999999999</v>
       </c>
       <c r="E4" s="4">
-        <v>5.2200000000000003E-2</v>
+        <v>5.1499999999999997E-2</v>
       </c>
       <c r="F4" s="11">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="G4" s="4">
-        <v>1E-4</v>
+        <v>2.0000000000000001E-4</v>
       </c>
       <c r="H4" s="9">
         <f t="shared" ref="H4:H27" si="0">+B4+D4+F4</f>
-        <v>0.49220000000000003</v>
+        <v>0.48170000000000002</v>
       </c>
       <c r="I4" s="5">
         <f t="shared" ref="I4:I18" si="1">+B4/$H4</f>
-        <v>0.27123120682649332</v>
+        <v>0.33693170022835789</v>
       </c>
       <c r="J4" s="5">
         <f t="shared" ref="J4:J18" si="2">+D4/H4</f>
-        <v>0.72815928484355952</v>
+        <v>0.6624455055013494</v>
       </c>
       <c r="K4" s="5">
         <f t="shared" ref="K4:K18" si="3">+F4/H4</f>
-        <v>6.0950832994717584E-4</v>
+        <v>6.2279427029271321E-4</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -2786,38 +2915,38 @@
         <v>3</v>
       </c>
       <c r="B5" s="13">
-        <v>1.0633999999999999</v>
+        <v>1.0328999999999999</v>
       </c>
       <c r="C5" s="4">
-        <v>0.15659999999999999</v>
+        <v>0.46100000000000002</v>
       </c>
       <c r="D5" s="11">
-        <v>2.69E-2</v>
+        <v>2.5100000000000001E-2</v>
       </c>
       <c r="E5" s="4">
-        <v>7.1000000000000004E-3</v>
+        <v>4.8999999999999998E-3</v>
       </c>
       <c r="F5" s="11">
-        <v>0.1171</v>
+        <v>0.11210000000000001</v>
       </c>
       <c r="G5" s="4">
-        <v>2.1100000000000001E-2</v>
+        <v>3.8699999999999998E-2</v>
       </c>
       <c r="H5" s="9">
         <f t="shared" si="0"/>
-        <v>1.2073999999999998</v>
+        <v>1.1700999999999999</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" si="1"/>
-        <v>0.88073546463475239</v>
+        <v>0.8827450645243996</v>
       </c>
       <c r="J5" s="5">
         <f t="shared" si="2"/>
-        <v>2.2279277786980294E-2</v>
+        <v>2.1451158020681996E-2</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" si="3"/>
-        <v>9.698525757826737E-2</v>
+        <v>9.5803777454918387E-2</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -2825,38 +2954,38 @@
         <v>4</v>
       </c>
       <c r="B6" s="13">
-        <v>0.17960000000000001</v>
+        <v>0.20080000000000001</v>
       </c>
       <c r="C6" s="4">
-        <v>4.24E-2</v>
+        <v>0.45650000000000002</v>
       </c>
       <c r="D6" s="11">
-        <v>2.8792</v>
+        <v>2.8708</v>
       </c>
       <c r="E6" s="4">
-        <v>0.434</v>
+        <v>0.51980000000000004</v>
       </c>
       <c r="F6" s="11">
-        <v>2.3534999999999999</v>
+        <v>2.3601999999999999</v>
       </c>
       <c r="G6" s="4">
-        <v>0.40620000000000001</v>
+        <v>0.38</v>
       </c>
       <c r="H6" s="9">
         <f t="shared" si="0"/>
-        <v>5.4123000000000001</v>
+        <v>5.4318</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" si="1"/>
-        <v>3.3183674223527894E-2</v>
+        <v>3.6967487757281196E-2</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="2"/>
-        <v>0.5319734678417678</v>
+        <v>0.52851725026694651</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" si="3"/>
-        <v>0.43484285793470429</v>
+        <v>0.43451526197577228</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -2864,38 +2993,38 @@
         <v>5</v>
       </c>
       <c r="B7" s="13">
-        <v>0.15340000000000001</v>
+        <v>0.17899999999999999</v>
       </c>
       <c r="C7" s="4">
-        <v>2.7E-2</v>
+        <v>0.38529999999999998</v>
       </c>
       <c r="D7" s="11">
-        <v>2.9999999999999997E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="E7" s="4">
-        <v>0</v>
+        <v>1.1999999999999999E-3</v>
       </c>
       <c r="F7" s="11">
-        <v>1.2999999999999999E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="G7" s="4">
-        <v>1.6000000000000001E-3</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="H7" s="9">
         <f t="shared" si="0"/>
-        <v>0.155</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="I7" s="5">
         <f t="shared" si="1"/>
-        <v>0.98967741935483877</v>
+        <v>0.98895027624309395</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="2"/>
-        <v>1.9354838709677417E-3</v>
+        <v>2.2099447513812156E-3</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" si="3"/>
-        <v>8.3870967741935479E-3</v>
+        <v>8.8397790055248626E-3</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -2903,38 +3032,38 @@
         <v>6</v>
       </c>
       <c r="B8" s="13">
-        <v>1.0084</v>
+        <v>1.0788</v>
       </c>
       <c r="C8" s="4">
-        <v>0.16159999999999999</v>
+        <v>0.45850000000000002</v>
       </c>
       <c r="D8" s="11">
-        <v>0.55189999999999995</v>
+        <v>0.58320000000000005</v>
       </c>
       <c r="E8" s="4">
-        <v>9.4200000000000006E-2</v>
+        <v>0.1802</v>
       </c>
       <c r="F8" s="11">
-        <v>0.32269999999999999</v>
+        <v>0.3619</v>
       </c>
       <c r="G8" s="4">
-        <v>5.8500000000000003E-2</v>
+        <v>0.122</v>
       </c>
       <c r="H8" s="9">
         <f t="shared" si="0"/>
-        <v>1.8829999999999998</v>
+        <v>2.0238999999999998</v>
       </c>
       <c r="I8" s="5">
         <f t="shared" si="1"/>
-        <v>0.53552841210833779</v>
+        <v>0.53303028805771036</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="2"/>
-        <v>0.29309612320764739</v>
+        <v>0.28815652947280007</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" si="3"/>
-        <v>0.17137546468401488</v>
+        <v>0.17881318246948963</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -2942,38 +3071,38 @@
         <v>7</v>
       </c>
       <c r="B9" s="13">
-        <v>4.1924000000000001</v>
+        <v>4.0505000000000004</v>
       </c>
       <c r="C9" s="4">
-        <v>0.90410000000000001</v>
+        <v>1.3262</v>
       </c>
       <c r="D9" s="11">
-        <v>1.3483000000000001</v>
+        <v>0.98199999999999998</v>
       </c>
       <c r="E9" s="4">
-        <v>0.29409999999999997</v>
+        <v>0.2472</v>
       </c>
       <c r="F9" s="11">
-        <v>9.1999999999999998E-3</v>
+        <v>9.1000000000000004E-3</v>
       </c>
       <c r="G9" s="4">
-        <v>3.3E-3</v>
+        <v>3.0999999999999999E-3</v>
       </c>
       <c r="H9" s="9">
         <f t="shared" si="0"/>
-        <v>5.5499000000000001</v>
+        <v>5.0416000000000007</v>
       </c>
       <c r="I9" s="5">
         <f t="shared" si="1"/>
-        <v>0.75540099821618412</v>
+        <v>0.80341558235480792</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="2"/>
-        <v>0.24294131425791457</v>
+        <v>0.19477943509996823</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" si="3"/>
-        <v>1.6576875259013675E-3</v>
+        <v>1.8049825452237382E-3</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -2981,38 +3110,38 @@
         <v>8</v>
       </c>
       <c r="B10" s="13">
-        <v>0.1449</v>
+        <v>0.17879999999999999</v>
       </c>
       <c r="C10" s="4">
-        <v>4.2799999999999998E-2</v>
+        <v>0.46379999999999999</v>
       </c>
       <c r="D10" s="11">
-        <v>1.29E-2</v>
+        <v>1.41E-2</v>
       </c>
       <c r="E10" s="4">
-        <v>3.3999999999999998E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="F10" s="11">
-        <v>0.52029999999999998</v>
+        <v>0.56230000000000002</v>
       </c>
       <c r="G10" s="4">
-        <v>0.1208</v>
+        <v>0.18720000000000001</v>
       </c>
       <c r="H10" s="9">
         <f t="shared" si="0"/>
-        <v>0.67809999999999993</v>
+        <v>0.75519999999999998</v>
       </c>
       <c r="I10" s="5">
         <f t="shared" si="1"/>
-        <v>0.21368529715381215</v>
+        <v>0.23675847457627117</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="2"/>
-        <v>1.9023742810794868E-2</v>
+        <v>1.8670550847457626E-2</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" si="3"/>
-        <v>0.7672909600353931</v>
+        <v>0.74457097457627119</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -3020,38 +3149,38 @@
         <v>9</v>
       </c>
       <c r="B11" s="13">
-        <v>0.13469999999999999</v>
+        <v>0.1368</v>
       </c>
       <c r="C11" s="4">
-        <v>5.0500000000000003E-2</v>
+        <v>0.40039999999999998</v>
       </c>
       <c r="D11" s="11">
-        <v>0.30220000000000002</v>
+        <v>0.27479999999999999</v>
       </c>
       <c r="E11" s="4">
-        <v>8.9499999999999996E-2</v>
+        <v>5.91E-2</v>
       </c>
       <c r="F11" s="11">
-        <v>7.7600000000000002E-2</v>
+        <v>5.7200000000000001E-2</v>
       </c>
       <c r="G11" s="4">
-        <v>2.3900000000000001E-2</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="H11" s="9">
         <f t="shared" si="0"/>
-        <v>0.51449999999999996</v>
+        <v>0.46879999999999999</v>
       </c>
       <c r="I11" s="5">
         <f t="shared" si="1"/>
-        <v>0.26180758017492711</v>
+        <v>0.29180887372013653</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="2"/>
-        <v>0.58736637512147727</v>
+        <v>0.58617747440273038</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" si="3"/>
-        <v>0.15082604470359573</v>
+        <v>0.1220136518771331</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -3059,38 +3188,38 @@
         <v>10</v>
       </c>
       <c r="B12" s="13">
-        <v>6.1499999999999999E-2</v>
+        <v>7.5300000000000006E-2</v>
       </c>
       <c r="C12" s="4">
-        <v>2.3E-2</v>
+        <v>0.2301</v>
       </c>
       <c r="D12" s="11">
-        <v>5.9999999999999995E-4</v>
+        <v>6.9999999999999999E-4</v>
       </c>
       <c r="E12" s="4">
-        <v>1E-4</v>
+        <v>1.2999999999999999E-3</v>
       </c>
       <c r="F12" s="11">
         <v>1.1000000000000001E-3</v>
       </c>
       <c r="G12" s="4">
-        <v>1.4E-3</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="H12" s="9">
         <f t="shared" si="0"/>
-        <v>6.3200000000000006E-2</v>
+        <v>7.7100000000000016E-2</v>
       </c>
       <c r="I12" s="5">
         <f t="shared" si="1"/>
-        <v>0.97310126582278467</v>
+        <v>0.97665369649805434</v>
       </c>
       <c r="J12" s="5">
         <f t="shared" si="2"/>
-        <v>9.4936708860759479E-3</v>
+        <v>9.0791180285343682E-3</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" si="3"/>
-        <v>1.740506329113924E-2</v>
+        <v>1.4267185473411152E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -3098,38 +3227,38 @@
         <v>11</v>
       </c>
       <c r="B13" s="13">
-        <v>0.15759999999999999</v>
+        <v>0.22070000000000001</v>
       </c>
       <c r="C13" s="4">
-        <v>6.0699999999999997E-2</v>
+        <v>0.74770000000000003</v>
       </c>
       <c r="D13" s="11">
-        <v>9.9281000000000006</v>
+        <v>9.7632999999999992</v>
       </c>
       <c r="E13" s="4">
-        <v>1.88</v>
+        <v>1.8113999999999999</v>
       </c>
       <c r="F13" s="11">
-        <v>22.502700000000001</v>
+        <v>22.0214</v>
       </c>
       <c r="G13" s="4">
-        <v>3.4729000000000001</v>
+        <v>2.7014</v>
       </c>
       <c r="H13" s="9">
         <f t="shared" si="0"/>
-        <v>32.5884</v>
+        <v>32.005400000000002</v>
       </c>
       <c r="I13" s="5">
         <f t="shared" si="1"/>
-        <v>4.8360766407678805E-3</v>
+        <v>6.8957113487099053E-3</v>
       </c>
       <c r="J13" s="5">
         <f t="shared" si="2"/>
-        <v>0.30465134833253554</v>
+        <v>0.3050516475344785</v>
       </c>
       <c r="K13" s="5">
         <f t="shared" si="3"/>
-        <v>0.69051257502669661</v>
+        <v>0.68805264111681153</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -3137,38 +3266,38 @@
         <v>12</v>
       </c>
       <c r="B14" s="13">
-        <v>0.10009999999999999</v>
+        <v>0.1273</v>
       </c>
       <c r="C14" s="4">
-        <v>2.1700000000000001E-2</v>
+        <v>0.4773</v>
       </c>
       <c r="D14" s="11">
+        <v>2.8E-3</v>
+      </c>
+      <c r="E14" s="4">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="F14" s="11">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="G14" s="4">
         <v>2.5999999999999999E-3</v>
-      </c>
-      <c r="E14" s="4">
-        <v>1.2999999999999999E-3</v>
-      </c>
-      <c r="F14" s="11">
-        <v>3.2000000000000002E-3</v>
-      </c>
-      <c r="G14" s="4">
-        <v>1.5E-3</v>
       </c>
       <c r="H14" s="9">
         <f t="shared" si="0"/>
-        <v>0.10589999999999999</v>
+        <v>0.13369999999999999</v>
       </c>
       <c r="I14" s="5">
         <f t="shared" si="1"/>
-        <v>0.94523135033050043</v>
+        <v>0.95213163799551237</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" si="2"/>
-        <v>2.4551463644948063E-2</v>
+        <v>2.0942408376963352E-2</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" si="3"/>
-        <v>3.0217186024551465E-2</v>
+        <v>2.6925953627524309E-2</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -3176,10 +3305,10 @@
         <v>13</v>
       </c>
       <c r="B15" s="13">
-        <v>5.9400000000000001E-2</v>
+        <v>7.1400000000000005E-2</v>
       </c>
       <c r="C15" s="4">
-        <v>1.6E-2</v>
+        <v>0.2354</v>
       </c>
       <c r="D15" s="11">
         <v>4.0000000000000002E-4</v>
@@ -3188,26 +3317,26 @@
         <v>1E-4</v>
       </c>
       <c r="F15" s="11">
-        <v>6.9999999999999999E-4</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="G15" s="4">
-        <v>1E-4</v>
+        <v>1.4E-3</v>
       </c>
       <c r="H15" s="9">
         <f t="shared" si="0"/>
-        <v>6.0499999999999998E-2</v>
+        <v>7.2599999999999998E-2</v>
       </c>
       <c r="I15" s="5">
         <f t="shared" si="1"/>
-        <v>0.98181818181818192</v>
+        <v>0.98347107438016534</v>
       </c>
       <c r="J15" s="5">
         <f t="shared" si="2"/>
-        <v>6.611570247933885E-3</v>
+        <v>5.5096418732782371E-3</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" si="3"/>
-        <v>1.1570247933884299E-2</v>
+        <v>1.1019283746556474E-2</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -3215,38 +3344,38 @@
         <v>14</v>
       </c>
       <c r="B16" s="13">
-        <v>0.16819999999999999</v>
+        <v>0.2868</v>
       </c>
       <c r="C16" s="4">
-        <v>4.4900000000000002E-2</v>
+        <v>1.1701999999999999</v>
       </c>
       <c r="D16" s="11">
-        <v>0.60680000000000001</v>
+        <v>0.61209999999999998</v>
       </c>
       <c r="E16" s="4">
-        <v>0.12540000000000001</v>
+        <v>0.1353</v>
       </c>
       <c r="F16" s="11">
-        <v>11.2263</v>
+        <v>11.4954</v>
       </c>
       <c r="G16" s="4">
-        <v>1.0256000000000001</v>
+        <v>1.3191999999999999</v>
       </c>
       <c r="H16" s="9">
         <f t="shared" si="0"/>
-        <v>12.001300000000001</v>
+        <v>12.394299999999999</v>
       </c>
       <c r="I16" s="5">
         <f t="shared" si="1"/>
-        <v>1.4015148358927781E-2</v>
+        <v>2.31396690414142E-2</v>
       </c>
       <c r="J16" s="5">
         <f t="shared" si="2"/>
-        <v>5.0561189204502845E-2</v>
+        <v>4.9385604673115868E-2</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="3"/>
-        <v>0.93542366243656938</v>
+        <v>0.92747472628547001</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -3254,38 +3383,38 @@
         <v>15</v>
       </c>
       <c r="B17" s="13">
-        <v>0.1973</v>
+        <v>0.65859999999999996</v>
       </c>
       <c r="C17" s="4">
-        <v>4.7500000000000001E-2</v>
+        <v>1.4416</v>
       </c>
       <c r="D17" s="11">
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="E17" s="4">
-        <v>5.9999999999999995E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="F17" s="11">
-        <v>876.95929999999998</v>
+        <v>874.42840000000001</v>
       </c>
       <c r="G17" s="4">
-        <v>19.710799999999999</v>
+        <v>22.526700000000002</v>
       </c>
       <c r="H17" s="9">
         <f t="shared" si="0"/>
-        <v>877.16210000000001</v>
+        <v>875.09249999999997</v>
       </c>
       <c r="I17" s="5">
         <f t="shared" si="1"/>
-        <v>2.2492991888272418E-4</v>
+        <v>7.5260615306381895E-4</v>
       </c>
       <c r="J17" s="5">
         <f t="shared" si="2"/>
-        <v>6.2702207493917022E-6</v>
+        <v>6.2850498661570063E-6</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" si="3"/>
-        <v>0.99976879986036782</v>
+        <v>0.99924110879707007</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -3293,38 +3422,38 @@
         <v>16</v>
       </c>
       <c r="B18" s="13">
-        <v>0.44519999999999998</v>
+        <v>0.48859999999999998</v>
       </c>
       <c r="C18" s="4">
-        <v>7.0000000000000007E-2</v>
+        <v>0.81499999999999995</v>
       </c>
       <c r="D18" s="11">
-        <v>0.15770000000000001</v>
+        <v>0.1474</v>
       </c>
       <c r="E18" s="4">
-        <v>2.07E-2</v>
+        <v>3.0800000000000001E-2</v>
       </c>
       <c r="F18" s="11">
-        <v>0.4556</v>
+        <v>0.46089999999999998</v>
       </c>
       <c r="G18" s="4">
-        <v>4.9099999999999998E-2</v>
+        <v>9.3700000000000006E-2</v>
       </c>
       <c r="H18" s="9">
         <f t="shared" si="0"/>
-        <v>1.0585</v>
+        <v>1.0969</v>
       </c>
       <c r="I18" s="5">
         <f t="shared" si="1"/>
-        <v>0.42059518186112421</v>
+        <v>0.44543714103382259</v>
       </c>
       <c r="J18" s="5">
         <f t="shared" si="2"/>
-        <v>0.14898441190363723</v>
+        <v>0.13437870361929075</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" si="3"/>
-        <v>0.43042040623523853</v>
+        <v>0.42018415534688669</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -3332,38 +3461,38 @@
         <v>17</v>
       </c>
       <c r="B19" s="13">
-        <v>0.16600000000000001</v>
+        <v>0.2293</v>
       </c>
       <c r="C19" s="4">
-        <v>2.9700000000000001E-2</v>
+        <v>0.69399999999999995</v>
       </c>
       <c r="D19" s="11">
-        <v>7.4382000000000001</v>
+        <v>7.3102999999999998</v>
       </c>
       <c r="E19" s="4">
-        <v>1.3631</v>
+        <v>1.4458</v>
       </c>
       <c r="F19" s="11">
-        <v>200.09180000000001</v>
+        <v>206.36789999999999</v>
       </c>
       <c r="G19" s="4">
-        <v>8.3059999999999992</v>
+        <v>7.2497999999999996</v>
       </c>
       <c r="H19" s="9">
         <f t="shared" si="0"/>
-        <v>207.696</v>
+        <v>213.9075</v>
       </c>
       <c r="I19" s="5">
         <f t="shared" ref="I19" si="4">+B19/$H19</f>
-        <v>7.9924505045836228E-4</v>
+        <v>1.0719586737257926E-3</v>
       </c>
       <c r="J19" s="5">
         <f t="shared" ref="J19" si="5">+D19/H19</f>
-        <v>3.5812918881442106E-2</v>
+        <v>3.4175052300643972E-2</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" ref="K19" si="6">+F19/H19</f>
-        <v>0.96338783606809952</v>
+        <v>0.96475298902563023</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -3371,165 +3500,312 @@
         <v>18</v>
       </c>
       <c r="B20" s="13">
-        <v>4.8099999999999997E-2</v>
+        <v>0.1077</v>
       </c>
       <c r="C20" s="4">
-        <v>1.72E-2</v>
+        <v>3.3799999999999997E-2</v>
       </c>
       <c r="D20" s="11">
-        <v>4.0000000000000002E-4</v>
+        <v>0.60599999999999998</v>
       </c>
       <c r="E20" s="4">
-        <v>1E-4</v>
+        <v>0.11459999999999999</v>
       </c>
       <c r="F20" s="11">
-        <v>4.0000000000000002E-4</v>
+        <v>0.60580000000000001</v>
       </c>
       <c r="G20" s="4">
-        <v>1E-4</v>
+        <v>0.12790000000000001</v>
       </c>
       <c r="H20" s="9">
         <f>+B20+D20+F20</f>
-        <v>4.8899999999999992E-2</v>
+        <v>1.3195000000000001</v>
       </c>
       <c r="I20" s="5">
         <f>+B20/$H20</f>
-        <v>0.98364008179959106</v>
+        <v>8.1621826449412654E-2</v>
       </c>
       <c r="J20" s="5">
         <f>+D20/H20</f>
-        <v>8.1799591002045015E-3</v>
+        <v>0.45926487305797647</v>
       </c>
       <c r="K20" s="5">
         <f>+F20/H20</f>
-        <v>8.1799591002045015E-3</v>
+        <v>0.45911330049261079</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="4"/>
+      <c r="B21" s="13">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C21" s="4">
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="D21" s="11">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E21" s="4">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="F21" s="11">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="G21" s="4">
+        <v>1.2999999999999999E-3</v>
+      </c>
       <c r="H21" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
+        <v>4.5799999999999993E-2</v>
+      </c>
+      <c r="I21" s="5">
+        <f>+B21/$H21</f>
+        <v>0.98253275109170313</v>
+      </c>
+      <c r="J21" s="5">
+        <f>+D21/H21</f>
+        <v>8.7336244541484729E-3</v>
+      </c>
+      <c r="K21" s="5">
+        <f>+F21/H21</f>
+        <v>8.7336244541484729E-3</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="4"/>
+      <c r="B22" s="13">
+        <v>4.7399999999999998E-2</v>
+      </c>
+      <c r="C22" s="4">
+        <v>1.9900000000000001E-2</v>
+      </c>
+      <c r="D22" s="11">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E22" s="4">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="F22" s="11">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="G22" s="4">
+        <v>1E-4</v>
+      </c>
       <c r="H22" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
+        <v>4.8099999999999997E-2</v>
+      </c>
+      <c r="I22" s="5">
+        <f t="shared" ref="I22:I27" si="7">+B22/$H22</f>
+        <v>0.9854469854469855</v>
+      </c>
+      <c r="J22" s="5">
+        <f t="shared" ref="J22:J27" si="8">+D22/H22</f>
+        <v>8.3160083160083165E-3</v>
+      </c>
+      <c r="K22" s="5">
+        <f t="shared" ref="K22:K27" si="9">+F22/H22</f>
+        <v>6.2370062370062365E-3</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="4"/>
+      <c r="B23" s="13">
+        <v>4.7300000000000002E-2</v>
+      </c>
+      <c r="C23" s="4">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="D23" s="11">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E23" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="F23" s="11">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="G23" s="4">
+        <v>4.0000000000000002E-4</v>
+      </c>
       <c r="H23" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
+        <v>4.8099999999999997E-2</v>
+      </c>
+      <c r="I23" s="5">
+        <f t="shared" si="7"/>
+        <v>0.98336798336798348</v>
+      </c>
+      <c r="J23" s="5">
+        <f t="shared" si="8"/>
+        <v>8.3160083160083165E-3</v>
+      </c>
+      <c r="K23" s="5">
+        <f t="shared" si="9"/>
+        <v>8.3160083160083165E-3</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>22</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="4"/>
+      <c r="B24" s="13">
+        <v>4.9399999999999999E-2</v>
+      </c>
+      <c r="C24" s="4">
+        <v>2.6100000000000002E-2</v>
+      </c>
+      <c r="D24" s="11">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="F24" s="11">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="G24" s="4">
+        <v>1E-4</v>
+      </c>
       <c r="H24" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
-      <c r="K24" s="5"/>
+        <v>0.05</v>
+      </c>
+      <c r="I24" s="5">
+        <f t="shared" si="7"/>
+        <v>0.98799999999999999</v>
+      </c>
+      <c r="J24" s="5">
+        <f t="shared" si="8"/>
+        <v>5.9999999999999993E-3</v>
+      </c>
+      <c r="K24" s="5">
+        <f t="shared" si="9"/>
+        <v>5.9999999999999993E-3</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>23</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="4"/>
+      <c r="B25" s="13">
+        <v>4.58E-2</v>
+      </c>
+      <c r="C25" s="4">
+        <v>2.01E-2</v>
+      </c>
+      <c r="D25" s="11">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E25" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="F25" s="11">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="G25" s="4">
+        <v>6.9999999999999999E-4</v>
+      </c>
       <c r="H25" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
-      <c r="K25" s="5"/>
+        <v>4.65E-2</v>
+      </c>
+      <c r="I25" s="5">
+        <f t="shared" si="7"/>
+        <v>0.98494623655913982</v>
+      </c>
+      <c r="J25" s="5">
+        <f t="shared" si="8"/>
+        <v>6.4516129032258056E-3</v>
+      </c>
+      <c r="K25" s="5">
+        <f t="shared" si="9"/>
+        <v>8.6021505376344086E-3</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>24</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="11"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="4"/>
+      <c r="B26" s="13">
+        <v>6.0400000000000002E-2</v>
+      </c>
+      <c r="C26" s="4">
+        <v>2.9600000000000001E-2</v>
+      </c>
+      <c r="D26" s="11">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E26" s="4">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F26" s="11">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G26" s="4">
+        <v>6.9999999999999999E-4</v>
+      </c>
       <c r="H26" s="9">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
-      <c r="K26" s="5"/>
+        <v>6.1400000000000003E-2</v>
+      </c>
+      <c r="I26" s="5">
+        <f t="shared" si="7"/>
+        <v>0.98371335504885993</v>
+      </c>
+      <c r="J26" s="5">
+        <f t="shared" si="8"/>
+        <v>8.1433224755700327E-3</v>
+      </c>
+      <c r="K26" s="5">
+        <f t="shared" si="9"/>
+        <v>8.1433224755700327E-3</v>
+      </c>
     </row>
     <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="15">
         <v>25</v>
       </c>
-      <c r="B27" s="17"/>
-      <c r="C27" s="18"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="18"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="18"/>
+      <c r="B27" s="17">
+        <v>5.1499999999999997E-2</v>
+      </c>
+      <c r="C27" s="18">
+        <v>1.9800000000000002E-2</v>
+      </c>
+      <c r="D27" s="19">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E27" s="18">
+        <v>1E-4</v>
+      </c>
+      <c r="F27" s="19">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="G27" s="18">
+        <v>1E-4</v>
+      </c>
       <c r="H27" s="20">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I27" s="21"/>
-      <c r="J27" s="21"/>
-      <c r="K27" s="21"/>
+        <v>5.2299999999999992E-2</v>
+      </c>
+      <c r="I27" s="21">
+        <f t="shared" si="7"/>
+        <v>0.98470363288718943</v>
+      </c>
+      <c r="J27" s="21">
+        <f t="shared" si="8"/>
+        <v>7.6481835564053552E-3</v>
+      </c>
+      <c r="K27" s="21">
+        <f t="shared" si="9"/>
+        <v>7.6481835564053552E-3</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
@@ -3550,34 +3826,34 @@
       </c>
       <c r="B29" s="13">
         <f>+AVERAGE(B3:B27)</f>
-        <v>0.47193888888888885</v>
+        <v>0.38901600000000003</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="11">
         <f>+AVERAGE(D3:D27)</f>
-        <v>1.3131999999999999</v>
+        <v>0.94149999999999978</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="11">
         <f>+AVERAGE(F3:F27)</f>
-        <v>61.986877777777778</v>
+        <v>44.795991999999984</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="9">
         <f>+SUM(H3:H27)</f>
-        <v>1147.8962999999999</v>
+        <v>1153.1627000000001</v>
       </c>
       <c r="I29" s="7">
         <f>+AVERAGE(I3:I27)</f>
-        <v>0.46289544596086035</v>
+        <v>0.58219525020818363</v>
       </c>
       <c r="J29" s="7">
-        <f t="shared" ref="J29:K29" si="7">+AVERAGE(J3:J27)</f>
-        <v>0.16831870227372117</v>
+        <f t="shared" ref="J29:K29" si="10">+AVERAGE(J3:J27)</f>
+        <v>0.13553326036613897</v>
       </c>
       <c r="K29" s="7">
-        <f t="shared" si="7"/>
-        <v>0.36878585176541839</v>
+        <f t="shared" si="10"/>
+        <v>0.28227148942567731</v>
       </c>
       <c r="L29" s="2"/>
     </row>
@@ -3587,17 +3863,17 @@
       </c>
       <c r="B30" s="13">
         <f>+MEDIAN(B3:B27)</f>
-        <v>0.1555</v>
+        <v>0.1368</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="11">
         <f>+MEDIAN(D3:D27)</f>
-        <v>9.2299999999999993E-2</v>
+        <v>1.41E-2</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="11">
         <f>+MEDIAN(F3:F27)</f>
-        <v>0.21989999999999998</v>
+        <v>9.1000000000000004E-3</v>
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="9"/>
@@ -3657,4 +3933,594 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E600A915-E6BE-496F-B7D8-4B3CDBED6E0D}">
+  <dimension ref="A1:G25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="B1:G25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="C1">
+        <v>0.46389999999999998</v>
+      </c>
+      <c r="D1">
+        <v>1.6799999999999999E-2</v>
+      </c>
+      <c r="E1">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="F1">
+        <v>1.0470999999999999</v>
+      </c>
+      <c r="G1">
+        <v>0.1457</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>0.1623</v>
+      </c>
+      <c r="C2">
+        <v>0.44629999999999997</v>
+      </c>
+      <c r="D2">
+        <v>0.31909999999999999</v>
+      </c>
+      <c r="E2">
+        <v>5.1499999999999997E-2</v>
+      </c>
+      <c r="F2">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="G2">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>1.0328999999999999</v>
+      </c>
+      <c r="C3">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="D3">
+        <v>2.5100000000000001E-2</v>
+      </c>
+      <c r="E3">
+        <v>4.8999999999999998E-3</v>
+      </c>
+      <c r="F3">
+        <v>0.11210000000000001</v>
+      </c>
+      <c r="G3">
+        <v>3.8699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>0.20080000000000001</v>
+      </c>
+      <c r="C4">
+        <v>0.45650000000000002</v>
+      </c>
+      <c r="D4">
+        <v>2.8708</v>
+      </c>
+      <c r="E4">
+        <v>0.51980000000000004</v>
+      </c>
+      <c r="F4">
+        <v>2.3601999999999999</v>
+      </c>
+      <c r="G4">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>0.17899999999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.38529999999999998</v>
+      </c>
+      <c r="D5">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E5">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="F5">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="G5">
+        <v>2.5000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>1.0788</v>
+      </c>
+      <c r="C6">
+        <v>0.45850000000000002</v>
+      </c>
+      <c r="D6">
+        <v>0.58320000000000005</v>
+      </c>
+      <c r="E6">
+        <v>0.1802</v>
+      </c>
+      <c r="F6">
+        <v>0.3619</v>
+      </c>
+      <c r="G6">
+        <v>0.122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>4.0505000000000004</v>
+      </c>
+      <c r="C7">
+        <v>1.3262</v>
+      </c>
+      <c r="D7">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="E7">
+        <v>0.2472</v>
+      </c>
+      <c r="F7">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="G7">
+        <v>3.0999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>0.17879999999999999</v>
+      </c>
+      <c r="C8">
+        <v>0.46379999999999999</v>
+      </c>
+      <c r="D8">
+        <v>1.41E-2</v>
+      </c>
+      <c r="E8">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="F8">
+        <v>0.56230000000000002</v>
+      </c>
+      <c r="G8">
+        <v>0.18720000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>0.1368</v>
+      </c>
+      <c r="C9">
+        <v>0.40039999999999998</v>
+      </c>
+      <c r="D9">
+        <v>0.27479999999999999</v>
+      </c>
+      <c r="E9">
+        <v>5.91E-2</v>
+      </c>
+      <c r="F9">
+        <v>5.7200000000000001E-2</v>
+      </c>
+      <c r="G9">
+        <v>1.2699999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>7.5300000000000006E-2</v>
+      </c>
+      <c r="C10">
+        <v>0.2301</v>
+      </c>
+      <c r="D10">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="E10">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="F10">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="G10">
+        <v>8.9999999999999998E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>0.22070000000000001</v>
+      </c>
+      <c r="C11">
+        <v>0.74770000000000003</v>
+      </c>
+      <c r="D11">
+        <v>9.7632999999999992</v>
+      </c>
+      <c r="E11">
+        <v>1.8113999999999999</v>
+      </c>
+      <c r="F11">
+        <v>22.0214</v>
+      </c>
+      <c r="G11">
+        <v>2.7014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>0.1273</v>
+      </c>
+      <c r="C12">
+        <v>0.4773</v>
+      </c>
+      <c r="D12">
+        <v>2.8E-3</v>
+      </c>
+      <c r="E12">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="F12">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="G12">
+        <v>2.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>7.1400000000000005E-2</v>
+      </c>
+      <c r="C13">
+        <v>0.2354</v>
+      </c>
+      <c r="D13">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E13">
+        <v>1E-4</v>
+      </c>
+      <c r="F13">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="G13">
+        <v>1.4E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>0.2868</v>
+      </c>
+      <c r="C14">
+        <v>1.1701999999999999</v>
+      </c>
+      <c r="D14">
+        <v>0.61209999999999998</v>
+      </c>
+      <c r="E14">
+        <v>0.1353</v>
+      </c>
+      <c r="F14">
+        <v>11.4954</v>
+      </c>
+      <c r="G14">
+        <v>1.3191999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>0.65859999999999996</v>
+      </c>
+      <c r="C15">
+        <v>1.4416</v>
+      </c>
+      <c r="D15">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="E15">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="F15">
+        <v>874.42840000000001</v>
+      </c>
+      <c r="G15">
+        <v>22.526700000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>0.48859999999999998</v>
+      </c>
+      <c r="C16">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="D16">
+        <v>0.1474</v>
+      </c>
+      <c r="E16">
+        <v>3.0800000000000001E-2</v>
+      </c>
+      <c r="F16">
+        <v>0.46089999999999998</v>
+      </c>
+      <c r="G16">
+        <v>9.3700000000000006E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>0.2293</v>
+      </c>
+      <c r="C17">
+        <v>0.69399999999999995</v>
+      </c>
+      <c r="D17">
+        <v>7.3102999999999998</v>
+      </c>
+      <c r="E17">
+        <v>1.4458</v>
+      </c>
+      <c r="F17">
+        <v>206.36789999999999</v>
+      </c>
+      <c r="G17">
+        <v>7.2497999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>0.1077</v>
+      </c>
+      <c r="C18">
+        <v>3.3799999999999997E-2</v>
+      </c>
+      <c r="D18">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="E18">
+        <v>0.11459999999999999</v>
+      </c>
+      <c r="F18">
+        <v>0.60580000000000001</v>
+      </c>
+      <c r="G18">
+        <v>0.12790000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C19">
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="D19">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E19">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="F19">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="G19">
+        <v>1.2999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>4.7399999999999998E-2</v>
+      </c>
+      <c r="C20">
+        <v>1.9900000000000001E-2</v>
+      </c>
+      <c r="D20">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E20">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="F20">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="G20">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>4.7300000000000002E-2</v>
+      </c>
+      <c r="C21">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="D21">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E21">
+        <v>1E-4</v>
+      </c>
+      <c r="F21">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="G21">
+        <v>4.0000000000000002E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>22</v>
+      </c>
+      <c r="B22">
+        <v>4.9399999999999999E-2</v>
+      </c>
+      <c r="C22">
+        <v>2.6100000000000002E-2</v>
+      </c>
+      <c r="D22">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E22">
+        <v>1E-4</v>
+      </c>
+      <c r="F22">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="G22">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>23</v>
+      </c>
+      <c r="B23">
+        <v>4.58E-2</v>
+      </c>
+      <c r="C23">
+        <v>2.01E-2</v>
+      </c>
+      <c r="D23">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E23">
+        <v>1E-4</v>
+      </c>
+      <c r="F23">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="G23">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>24</v>
+      </c>
+      <c r="B24">
+        <v>6.0400000000000002E-2</v>
+      </c>
+      <c r="C24">
+        <v>2.9600000000000001E-2</v>
+      </c>
+      <c r="D24">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E24">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F24">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G24">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>5.1499999999999997E-2</v>
+      </c>
+      <c r="C25">
+        <v>1.9800000000000002E-2</v>
+      </c>
+      <c r="D25">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E25">
+        <v>1E-4</v>
+      </c>
+      <c r="F25">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="G25">
+        <v>1E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the analysis after day 19
</commit_message>
<xml_diff>
--- a/2020/analysis/execution times.xlsx
+++ b/2020/analysis/execution times.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\arno\git\AdventOfCode\2020\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6372E6F-4EA8-45E1-A3C1-6901847A1245}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC5CAC23-E640-4579-8C55-D8F4167BBC8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{23AEBC82-DD3C-489D-BC2D-D322F6541D25}"/>
   </bookViews>
   <sheets>
     <sheet name="analysis" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -613,10 +614,10 @@
                     <c:v>0.69399999999999995</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>3.3799999999999997E-2</c:v>
+                    <c:v>0.1479</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>1.5800000000000002E-2</c:v>
+                    <c:v>9.2100000000000001E-2</c:v>
                   </c:pt>
                   <c:pt idx="19">
                     <c:v>1.9900000000000001E-2</c:v>
@@ -697,10 +698,10 @@
                     <c:v>0.69399999999999995</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>3.3799999999999997E-2</c:v>
+                    <c:v>0.1479</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>1.5800000000000002E-2</c:v>
+                    <c:v>9.2100000000000001E-2</c:v>
                   </c:pt>
                   <c:pt idx="19">
                     <c:v>1.9900000000000001E-2</c:v>
@@ -739,10 +740,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$A$3:$A$20</c:f>
+              <c:f>analysis!$A$3:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -796,16 +797,19 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$B$3:$B$20</c:f>
+              <c:f>analysis!$B$3:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>9.2999999999999999E-2</c:v>
                 </c:pt>
@@ -858,7 +862,10 @@
                   <c:v>0.2293</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.1077</c:v>
+                  <c:v>0.67469999999999997</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.53159999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -955,10 +962,10 @@
                     <c:v>1.4458</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>0.11459999999999999</c:v>
+                    <c:v>3.3099999999999997E-2</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>1.1999999999999999E-3</c:v>
+                    <c:v>30.326699999999999</c:v>
                   </c:pt>
                   <c:pt idx="19">
                     <c:v>1.2999999999999999E-3</c:v>
@@ -1039,10 +1046,10 @@
                     <c:v>1.4458</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>0.11459999999999999</c:v>
+                    <c:v>3.3099999999999997E-2</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>1.1999999999999999E-3</c:v>
+                    <c:v>30.326699999999999</c:v>
                   </c:pt>
                   <c:pt idx="19">
                     <c:v>1.2999999999999999E-3</c:v>
@@ -1081,10 +1088,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$A$3:$A$20</c:f>
+              <c:f>analysis!$A$3:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1138,16 +1145,19 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$D$3:$D$20</c:f>
+              <c:f>analysis!$D$3:$D$21</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>1.6799999999999999E-2</c:v>
                 </c:pt>
@@ -1200,7 +1210,10 @@
                   <c:v>7.3102999999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.60599999999999998</c:v>
+                  <c:v>0.1293</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2239.6855</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1297,10 +1310,10 @@
                     <c:v>7.2497999999999996</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>0.12790000000000001</c:v>
+                    <c:v>2.75E-2</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>1.2999999999999999E-3</c:v>
+                    <c:v>51.3491</c:v>
                   </c:pt>
                   <c:pt idx="19">
                     <c:v>1E-4</c:v>
@@ -1381,10 +1394,10 @@
                     <c:v>7.2497999999999996</c:v>
                   </c:pt>
                   <c:pt idx="17">
-                    <c:v>0.12790000000000001</c:v>
+                    <c:v>2.75E-2</c:v>
                   </c:pt>
                   <c:pt idx="18">
-                    <c:v>1.2999999999999999E-3</c:v>
+                    <c:v>51.3491</c:v>
                   </c:pt>
                   <c:pt idx="19">
                     <c:v>1E-4</c:v>
@@ -1423,10 +1436,10 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>analysis!$A$3:$A$20</c:f>
+              <c:f>analysis!$A$3:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1480,16 +1493,19 @@
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>analysis!$F$3:$F$20</c:f>
+              <c:f>analysis!$F$3:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="19"/>
                 <c:pt idx="0">
                   <c:v>1.0470999999999999</c:v>
                 </c:pt>
@@ -1542,7 +1558,10 @@
                   <c:v>206.36789999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.60580000000000001</c:v>
+                  <c:v>0.12859999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3070.2143999999998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2774,7 +2793,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3500,38 +3519,38 @@
         <v>18</v>
       </c>
       <c r="B20" s="13">
-        <v>0.1077</v>
+        <v>0.67469999999999997</v>
       </c>
       <c r="C20" s="4">
-        <v>3.3799999999999997E-2</v>
+        <v>0.1479</v>
       </c>
       <c r="D20" s="11">
-        <v>0.60599999999999998</v>
+        <v>0.1293</v>
       </c>
       <c r="E20" s="4">
-        <v>0.11459999999999999</v>
+        <v>3.3099999999999997E-2</v>
       </c>
       <c r="F20" s="11">
-        <v>0.60580000000000001</v>
+        <v>0.12859999999999999</v>
       </c>
       <c r="G20" s="4">
-        <v>0.12790000000000001</v>
+        <v>2.75E-2</v>
       </c>
       <c r="H20" s="9">
         <f>+B20+D20+F20</f>
-        <v>1.3195000000000001</v>
+        <v>0.93259999999999987</v>
       </c>
       <c r="I20" s="5">
         <f>+B20/$H20</f>
-        <v>8.1621826449412654E-2</v>
+        <v>0.72346129101436851</v>
       </c>
       <c r="J20" s="5">
         <f>+D20/H20</f>
-        <v>0.45926487305797647</v>
+        <v>0.1386446493673601</v>
       </c>
       <c r="K20" s="5">
         <f>+F20/H20</f>
-        <v>0.45911330049261079</v>
+        <v>0.1378940596182715</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -3539,38 +3558,38 @@
         <v>19</v>
       </c>
       <c r="B21" s="13">
-        <v>4.4999999999999998E-2</v>
+        <v>0.53159999999999996</v>
       </c>
       <c r="C21" s="4">
-        <v>1.5800000000000002E-2</v>
+        <v>9.2100000000000001E-2</v>
       </c>
       <c r="D21" s="11">
-        <v>4.0000000000000002E-4</v>
+        <v>2239.6855</v>
       </c>
       <c r="E21" s="4">
-        <v>1.1999999999999999E-3</v>
+        <v>30.326699999999999</v>
       </c>
       <c r="F21" s="11">
-        <v>4.0000000000000002E-4</v>
+        <v>3070.2143999999998</v>
       </c>
       <c r="G21" s="4">
-        <v>1.2999999999999999E-3</v>
+        <v>51.3491</v>
       </c>
       <c r="H21" s="9">
         <f t="shared" si="0"/>
-        <v>4.5799999999999993E-2</v>
+        <v>5310.4314999999997</v>
       </c>
       <c r="I21" s="5">
         <f>+B21/$H21</f>
-        <v>0.98253275109170313</v>
+        <v>1.0010485965217704E-4</v>
       </c>
       <c r="J21" s="5">
         <f>+D21/H21</f>
-        <v>8.7336244541484729E-3</v>
+        <v>0.42175207419585398</v>
       </c>
       <c r="K21" s="5">
         <f>+F21/H21</f>
-        <v>8.7336244541484729E-3</v>
+        <v>0.57814782094449391</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -3826,34 +3845,34 @@
       </c>
       <c r="B29" s="13">
         <f>+AVERAGE(B3:B27)</f>
-        <v>0.38901600000000003</v>
+        <v>0.43115999999999999</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="11">
         <f>+AVERAGE(D3:D27)</f>
-        <v>0.94149999999999978</v>
+        <v>90.509836000000007</v>
       </c>
       <c r="E29" s="4"/>
       <c r="F29" s="11">
         <f>+AVERAGE(F3:F27)</f>
-        <v>44.795991999999984</v>
+        <v>167.58546399999994</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="9">
         <f>+SUM(H3:H27)</f>
-        <v>1153.1627000000001</v>
+        <v>6463.1615000000002</v>
       </c>
       <c r="I29" s="7">
         <f>+AVERAGE(I3:I27)</f>
-        <v>0.58219525020818363</v>
+        <v>0.56857152294149982</v>
       </c>
       <c r="J29" s="7">
         <f t="shared" ref="J29:K29" si="10">+AVERAGE(J3:J27)</f>
-        <v>0.13553326036613897</v>
+        <v>0.13922918940818257</v>
       </c>
       <c r="K29" s="7">
         <f t="shared" si="10"/>
-        <v>0.28227148942567731</v>
+        <v>0.29219928765031761</v>
       </c>
       <c r="L29" s="2"/>
     </row>
@@ -3863,17 +3882,17 @@
       </c>
       <c r="B30" s="13">
         <f>+MEDIAN(B3:B27)</f>
-        <v>0.1368</v>
+        <v>0.17879999999999999</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="11">
         <f>+MEDIAN(D3:D27)</f>
-        <v>1.41E-2</v>
+        <v>1.6799999999999999E-2</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="11">
         <f>+MEDIAN(F3:F27)</f>
-        <v>9.1000000000000004E-3</v>
+        <v>5.7200000000000001E-2</v>
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="9"/>
@@ -3936,6 +3955,41 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE1959E-4818-4A5D-B3DD-EA9429A72965}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0.53159999999999996</v>
+      </c>
+      <c r="B1">
+        <v>9.2100000000000001E-2</v>
+      </c>
+      <c r="C1">
+        <v>2239.6855</v>
+      </c>
+      <c r="D1">
+        <v>30.326699999999999</v>
+      </c>
+      <c r="E1">
+        <v>3070.2143999999998</v>
+      </c>
+      <c r="F1">
+        <v>51.3491</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E600A915-E6BE-496F-B7D8-4B3CDBED6E0D}">
   <dimension ref="A1:G25"/>
   <sheetViews>

</xml_diff>